<commit_message>
altered the findings tracker in FOLDER/Mainfolder/... to ensure others can run ValidateTicketMapping.xaml
</commit_message>
<xml_diff>
--- a/FOLDER/Mainfolder/Daily_Change_Monitoring/Findings Tracker.xlsx
+++ b/FOLDER/Mainfolder/Daily_Change_Monitoring/Findings Tracker.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S\Documents\UiPath\Step_4\FOLDER\Mainfolder\Daily_Change_Monitoring\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S\Documents\UiPath_2\Robotic_Process_Automation\FOLDER\Mainfolder\Daily_Change_Monitoring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4083BA90-4E0F-496A-9C9C-175F4058A0D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AF54CFF-A8EE-4280-A2E9-F8C607B56FBF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="101">
   <si>
     <t>Date of Delta</t>
   </si>
@@ -315,19 +315,19 @@
     <t>\\MainFolder\Remediation_or_Justification Evidence\1-22-2020\RandomFolder2\</t>
   </si>
   <si>
-    <t>C:\Users\S\Documents\UiPath\Step_4\FOLDER\Mainfolder\Remediation_or_Justification Evidence\1-09-2020\RE: Random Email.msg</t>
-  </si>
-  <si>
-    <t>C:\Users\S\Documents\UiPath\Step_4\FOLDER\Mainfolder\Remediation_or_Justification Evidence\1-13-2020\CHR0000230943.pdf</t>
-  </si>
-  <si>
-    <t>C:\Users\S\Documents\UiPath\Step_4\FOLDER\Mainfolder\Remediation_or_Justification Evidence\1-13-2020\</t>
-  </si>
-  <si>
-    <t>C:\Users\S\Documents\UiPath\Step_4\FOLDER\Mainfolder\Remediation_or_Justification Evidence\1-14-2020\RE: Random Email.msg</t>
-  </si>
-  <si>
-    <t>C:\Users\S\Documents\UiPath\Step_4\FOLDER\Mainfolder\Remediation_or_Justification Evidence\1-14-2020\CHR0000291924.pdf</t>
+    <t>FOLDER\Mainfolder\Remediation_or_Justification Evidence\1-09-2020\RE: Random Email.msg</t>
+  </si>
+  <si>
+    <t>FOLDER\Mainfolder\Remediation_or_Justification Evidence\1-13-2020\CHR0000230943.pdf</t>
+  </si>
+  <si>
+    <t>FOLDER\Mainfolder\Remediation_or_Justification Evidence\1-13-2020\</t>
+  </si>
+  <si>
+    <t>FOLDER\Mainfolder\Remediation_or_Justification Evidence\1-14-2020\RE: Random Email.msg</t>
+  </si>
+  <si>
+    <t>FOLDER\Mainfolder\Remediation_or_Justification Evidence\1-14-2020\CHR0000291924.pdf</t>
   </si>
 </sst>
 </file>
@@ -698,7 +698,7 @@
   <dimension ref="A1:M120"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
got sections 1-3 to output correctly to the output file
</commit_message>
<xml_diff>
--- a/FOLDER/Mainfolder/Daily_Change_Monitoring/Findings Tracker.xlsx
+++ b/FOLDER/Mainfolder/Daily_Change_Monitoring/Findings Tracker.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S\Documents\UiPath_2\Robotic_Process_Automation\FOLDER\Mainfolder\Daily_Change_Monitoring\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1551b3744a113d45/Documents/UiPath/Robotic_Process_Automation/FOLDER/Mainfolder/Daily_Change_Monitoring/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AF54CFF-A8EE-4280-A2E9-F8C607B56FBF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FindingsTracker" sheetId="1" r:id="rId1"/>
@@ -701,24 +701,24 @@
       <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.81640625" customWidth="1"/>
-    <col min="2" max="2" width="15.1796875" customWidth="1"/>
-    <col min="3" max="3" width="15.453125" customWidth="1"/>
+    <col min="1" max="1" width="11.77734375" customWidth="1"/>
+    <col min="2" max="2" width="15.21875" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" customWidth="1"/>
     <col min="4" max="4" width="61" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.26953125" customWidth="1"/>
-    <col min="6" max="6" width="17.81640625" customWidth="1"/>
-    <col min="7" max="7" width="18.453125" customWidth="1"/>
+    <col min="5" max="5" width="21.21875" customWidth="1"/>
+    <col min="6" max="6" width="17.77734375" customWidth="1"/>
+    <col min="7" max="7" width="18.44140625" customWidth="1"/>
     <col min="8" max="8" width="22" customWidth="1"/>
-    <col min="9" max="9" width="21.453125" customWidth="1"/>
+    <col min="9" max="9" width="21.44140625" customWidth="1"/>
     <col min="10" max="10" width="11" customWidth="1"/>
     <col min="11" max="11" width="29" customWidth="1"/>
-    <col min="12" max="12" width="92.453125" customWidth="1"/>
+    <col min="12" max="12" width="92.44140625" customWidth="1"/>
     <col min="13" max="13" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="55.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" ht="54" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -759,7 +759,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
         <v>43839</v>
       </c>
@@ -800,7 +800,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8">
         <v>43839</v>
       </c>
@@ -841,7 +841,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8">
         <v>43839</v>
       </c>
@@ -882,7 +882,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
         <v>43839</v>
       </c>
@@ -923,7 +923,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8">
         <v>43843</v>
       </c>
@@ -964,7 +964,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
         <v>43843</v>
       </c>
@@ -1005,7 +1005,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
         <v>43843</v>
       </c>
@@ -1046,7 +1046,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
         <v>43844</v>
       </c>
@@ -1087,7 +1087,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="8">
         <v>43844</v>
       </c>
@@ -1128,7 +1128,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="8">
         <v>43852</v>
       </c>
@@ -1169,7 +1169,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="8">
         <v>43852</v>
       </c>
@@ -1210,7 +1210,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="8">
         <v>43852</v>
       </c>
@@ -1251,7 +1251,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="8">
         <v>43852</v>
       </c>
@@ -1292,7 +1292,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="8">
         <v>43854</v>
       </c>
@@ -1333,7 +1333,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8">
         <v>43854</v>
       </c>
@@ -1374,7 +1374,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="8">
         <v>43854</v>
       </c>
@@ -1415,7 +1415,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="12">
         <v>43885</v>
       </c>
@@ -1432,7 +1432,7 @@
       <c r="L18" s="5"/>
       <c r="M18" s="2"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="12">
         <v>43489</v>
       </c>
@@ -1449,7 +1449,7 @@
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -1464,7 +1464,7 @@
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -1478,7 +1478,7 @@
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -1492,7 +1492,7 @@
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -1506,7 +1506,7 @@
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -1520,7 +1520,7 @@
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -1534,7 +1534,7 @@
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -1548,7 +1548,7 @@
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -1562,7 +1562,7 @@
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -1576,7 +1576,7 @@
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -1590,7 +1590,7 @@
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -1604,7 +1604,7 @@
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -1618,7 +1618,7 @@
       <c r="K31" s="2"/>
       <c r="L31" s="2"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -1632,7 +1632,7 @@
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -1646,7 +1646,7 @@
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -1660,7 +1660,7 @@
       <c r="K34" s="2"/>
       <c r="L34" s="2"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -1674,7 +1674,7 @@
       <c r="K35" s="2"/>
       <c r="L35" s="2"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -1688,7 +1688,7 @@
       <c r="K36" s="2"/>
       <c r="L36" s="2"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -1702,7 +1702,7 @@
       <c r="K37" s="2"/>
       <c r="L37" s="2"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -1716,7 +1716,7 @@
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -1730,7 +1730,7 @@
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -1744,7 +1744,7 @@
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -1758,7 +1758,7 @@
       <c r="K41" s="2"/>
       <c r="L41" s="2"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -1772,7 +1772,7 @@
       <c r="K42" s="2"/>
       <c r="L42" s="2"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -1786,7 +1786,7 @@
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -1800,7 +1800,7 @@
       <c r="K44" s="2"/>
       <c r="L44" s="2"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -1814,7 +1814,7 @@
       <c r="K45" s="2"/>
       <c r="L45" s="2"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -1828,7 +1828,7 @@
       <c r="K46" s="2"/>
       <c r="L46" s="2"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -1842,7 +1842,7 @@
       <c r="K47" s="2"/>
       <c r="L47" s="2"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -1856,7 +1856,7 @@
       <c r="K48" s="2"/>
       <c r="L48" s="2"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -1870,7 +1870,7 @@
       <c r="K49" s="2"/>
       <c r="L49" s="2"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
@@ -1884,7 +1884,7 @@
       <c r="K50" s="2"/>
       <c r="L50" s="2"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
@@ -1898,7 +1898,7 @@
       <c r="K51" s="2"/>
       <c r="L51" s="2"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
@@ -1912,7 +1912,7 @@
       <c r="K52" s="2"/>
       <c r="L52" s="2"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
@@ -1926,7 +1926,7 @@
       <c r="K53" s="2"/>
       <c r="L53" s="2"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
@@ -1940,7 +1940,7 @@
       <c r="K54" s="2"/>
       <c r="L54" s="2"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
@@ -1954,7 +1954,7 @@
       <c r="K55" s="2"/>
       <c r="L55" s="2"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
@@ -1968,7 +1968,7 @@
       <c r="K56" s="2"/>
       <c r="L56" s="2"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
@@ -1982,7 +1982,7 @@
       <c r="K57" s="2"/>
       <c r="L57" s="2"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
@@ -1996,7 +1996,7 @@
       <c r="K58" s="2"/>
       <c r="L58" s="2"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
@@ -2010,7 +2010,7 @@
       <c r="K59" s="2"/>
       <c r="L59" s="2"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
@@ -2024,7 +2024,7 @@
       <c r="K60" s="2"/>
       <c r="L60" s="2"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
@@ -2038,7 +2038,7 @@
       <c r="K61" s="2"/>
       <c r="L61" s="2"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
@@ -2052,7 +2052,7 @@
       <c r="K62" s="2"/>
       <c r="L62" s="2"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
@@ -2066,7 +2066,7 @@
       <c r="K63" s="2"/>
       <c r="L63" s="2"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
@@ -2080,7 +2080,7 @@
       <c r="K64" s="2"/>
       <c r="L64" s="2"/>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
@@ -2094,7 +2094,7 @@
       <c r="K65" s="2"/>
       <c r="L65" s="2"/>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
@@ -2108,7 +2108,7 @@
       <c r="K66" s="2"/>
       <c r="L66" s="2"/>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
@@ -2122,7 +2122,7 @@
       <c r="K67" s="2"/>
       <c r="L67" s="2"/>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
@@ -2136,7 +2136,7 @@
       <c r="K68" s="2"/>
       <c r="L68" s="2"/>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
@@ -2150,7 +2150,7 @@
       <c r="K69" s="2"/>
       <c r="L69" s="2"/>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A70" s="2"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
@@ -2164,7 +2164,7 @@
       <c r="K70" s="2"/>
       <c r="L70" s="2"/>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
@@ -2178,7 +2178,7 @@
       <c r="K71" s="2"/>
       <c r="L71" s="2"/>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
@@ -2192,7 +2192,7 @@
       <c r="K72" s="2"/>
       <c r="L72" s="2"/>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
@@ -2206,7 +2206,7 @@
       <c r="K73" s="2"/>
       <c r="L73" s="2"/>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
@@ -2220,7 +2220,7 @@
       <c r="K74" s="2"/>
       <c r="L74" s="2"/>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
@@ -2234,7 +2234,7 @@
       <c r="K75" s="2"/>
       <c r="L75" s="2"/>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
@@ -2248,7 +2248,7 @@
       <c r="K76" s="2"/>
       <c r="L76" s="2"/>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A77" s="2"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
@@ -2262,7 +2262,7 @@
       <c r="K77" s="2"/>
       <c r="L77" s="2"/>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A78" s="2"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
@@ -2276,7 +2276,7 @@
       <c r="K78" s="2"/>
       <c r="L78" s="2"/>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A79" s="2"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
@@ -2290,7 +2290,7 @@
       <c r="K79" s="2"/>
       <c r="L79" s="2"/>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A80" s="2"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
@@ -2304,7 +2304,7 @@
       <c r="K80" s="2"/>
       <c r="L80" s="2"/>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A81" s="2"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
@@ -2318,7 +2318,7 @@
       <c r="K81" s="2"/>
       <c r="L81" s="2"/>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
@@ -2332,7 +2332,7 @@
       <c r="K82" s="2"/>
       <c r="L82" s="2"/>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
@@ -2346,7 +2346,7 @@
       <c r="K83" s="2"/>
       <c r="L83" s="2"/>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A84" s="2"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
@@ -2360,7 +2360,7 @@
       <c r="K84" s="2"/>
       <c r="L84" s="2"/>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A85" s="2"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
@@ -2374,7 +2374,7 @@
       <c r="K85" s="2"/>
       <c r="L85" s="2"/>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A86" s="2"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
@@ -2388,7 +2388,7 @@
       <c r="K86" s="2"/>
       <c r="L86" s="2"/>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A87" s="2"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
@@ -2402,7 +2402,7 @@
       <c r="K87" s="2"/>
       <c r="L87" s="2"/>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A88" s="2"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
@@ -2416,7 +2416,7 @@
       <c r="K88" s="2"/>
       <c r="L88" s="2"/>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A89" s="2"/>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
@@ -2430,7 +2430,7 @@
       <c r="K89" s="2"/>
       <c r="L89" s="2"/>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A90" s="2"/>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
@@ -2444,7 +2444,7 @@
       <c r="K90" s="2"/>
       <c r="L90" s="2"/>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A91" s="2"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
@@ -2458,7 +2458,7 @@
       <c r="K91" s="2"/>
       <c r="L91" s="2"/>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A92" s="2"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
@@ -2472,7 +2472,7 @@
       <c r="K92" s="2"/>
       <c r="L92" s="2"/>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A93" s="2"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
@@ -2486,7 +2486,7 @@
       <c r="K93" s="2"/>
       <c r="L93" s="2"/>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A94" s="2"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
@@ -2500,7 +2500,7 @@
       <c r="K94" s="2"/>
       <c r="L94" s="2"/>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A95" s="2"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
@@ -2514,7 +2514,7 @@
       <c r="K95" s="2"/>
       <c r="L95" s="2"/>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A96" s="2"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
@@ -2528,7 +2528,7 @@
       <c r="K96" s="2"/>
       <c r="L96" s="2"/>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A97" s="2"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
@@ -2542,7 +2542,7 @@
       <c r="K97" s="2"/>
       <c r="L97" s="2"/>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A98" s="2"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
@@ -2556,7 +2556,7 @@
       <c r="K98" s="2"/>
       <c r="L98" s="2"/>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A99" s="2"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
@@ -2570,7 +2570,7 @@
       <c r="K99" s="2"/>
       <c r="L99" s="2"/>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A100" s="2"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
@@ -2584,7 +2584,7 @@
       <c r="K100" s="2"/>
       <c r="L100" s="2"/>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A101" s="2"/>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
@@ -2598,7 +2598,7 @@
       <c r="K101" s="2"/>
       <c r="L101" s="2"/>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A102" s="2"/>
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
@@ -2612,7 +2612,7 @@
       <c r="K102" s="2"/>
       <c r="L102" s="2"/>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A103" s="2"/>
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
@@ -2626,7 +2626,7 @@
       <c r="K103" s="2"/>
       <c r="L103" s="2"/>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A104" s="2"/>
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
@@ -2640,7 +2640,7 @@
       <c r="K104" s="2"/>
       <c r="L104" s="2"/>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A105" s="2"/>
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
@@ -2654,7 +2654,7 @@
       <c r="K105" s="2"/>
       <c r="L105" s="2"/>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A106" s="2"/>
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
@@ -2668,7 +2668,7 @@
       <c r="K106" s="2"/>
       <c r="L106" s="2"/>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A107" s="2"/>
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
@@ -2682,7 +2682,7 @@
       <c r="K107" s="2"/>
       <c r="L107" s="2"/>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A108" s="2"/>
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
@@ -2696,7 +2696,7 @@
       <c r="K108" s="2"/>
       <c r="L108" s="2"/>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A109" s="2"/>
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
@@ -2710,7 +2710,7 @@
       <c r="K109" s="2"/>
       <c r="L109" s="2"/>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A110" s="2"/>
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
@@ -2724,7 +2724,7 @@
       <c r="K110" s="2"/>
       <c r="L110" s="2"/>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A111" s="2"/>
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
@@ -2738,7 +2738,7 @@
       <c r="K111" s="2"/>
       <c r="L111" s="2"/>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A112" s="2"/>
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
@@ -2752,7 +2752,7 @@
       <c r="K112" s="2"/>
       <c r="L112" s="2"/>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A113" s="2"/>
       <c r="B113" s="2"/>
       <c r="C113" s="2"/>
@@ -2766,7 +2766,7 @@
       <c r="K113" s="2"/>
       <c r="L113" s="2"/>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A114" s="2"/>
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
@@ -2780,7 +2780,7 @@
       <c r="K114" s="2"/>
       <c r="L114" s="2"/>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A115" s="2"/>
       <c r="B115" s="2"/>
       <c r="C115" s="2"/>
@@ -2794,7 +2794,7 @@
       <c r="K115" s="2"/>
       <c r="L115" s="2"/>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A116" s="2"/>
       <c r="B116" s="2"/>
       <c r="C116" s="2"/>
@@ -2808,7 +2808,7 @@
       <c r="K116" s="2"/>
       <c r="L116" s="2"/>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A117" s="2"/>
       <c r="B117" s="2"/>
       <c r="C117" s="2"/>
@@ -2822,7 +2822,7 @@
       <c r="K117" s="2"/>
       <c r="L117" s="2"/>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A118" s="2"/>
       <c r="B118" s="2"/>
       <c r="C118" s="2"/>
@@ -2836,7 +2836,7 @@
       <c r="K118" s="2"/>
       <c r="L118" s="2"/>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A119" s="2"/>
       <c r="B119" s="2"/>
       <c r="C119" s="2"/>
@@ -2850,7 +2850,7 @@
       <c r="K119" s="2"/>
       <c r="L119" s="2"/>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A120" s="2"/>
       <c r="B120" s="2"/>
       <c r="C120" s="2"/>

</xml_diff>

<commit_message>
adding pdfs with output
</commit_message>
<xml_diff>
--- a/FOLDER/Mainfolder/Daily_Change_Monitoring/Findings Tracker.xlsx
+++ b/FOLDER/Mainfolder/Daily_Change_Monitoring/Findings Tracker.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natha\Documents\UiPath\Robotic_Process_Automation\FOLDER\Mainfolder\Daily_Change_Monitoring\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1551b3744a113d45/Documents/UiPath/Robotic_Process_Automation/FOLDER/Mainfolder/Daily_Change_Monitoring/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5791B0D-0F90-4505-86CA-5D0F1618DA32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="114_{8AB96BB5-B659-4EAD-A8B6-E1AFCAECE06F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5775" yWindow="8475" windowWidth="25590" windowHeight="12660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4008" yWindow="2256" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FindingsTracker" sheetId="1" r:id="rId1"/>
@@ -695,24 +695,24 @@
       <selection activeCell="M2" sqref="M2:M17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" customWidth="1"/>
     <col min="4" max="4" width="61" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.28515625" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" customWidth="1"/>
-    <col min="7" max="7" width="18.42578125" customWidth="1"/>
+    <col min="5" max="5" width="21.33203125" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" customWidth="1"/>
+    <col min="7" max="7" width="18.44140625" customWidth="1"/>
     <col min="8" max="8" width="22" customWidth="1"/>
-    <col min="9" max="9" width="21.42578125" customWidth="1"/>
+    <col min="9" max="9" width="21.44140625" customWidth="1"/>
     <col min="10" max="10" width="11" customWidth="1"/>
     <col min="11" max="11" width="29" customWidth="1"/>
-    <col min="12" max="12" width="92.42578125" customWidth="1"/>
+    <col min="12" max="12" width="92.44140625" customWidth="1"/>
     <col min="13" max="13" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="56.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="54" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -753,7 +753,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
         <v>43839</v>
       </c>
@@ -792,7 +792,7 @@
       </c>
       <c r="M2" s="10"/>
     </row>
-    <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8">
         <v>43839</v>
       </c>
@@ -831,7 +831,7 @@
       </c>
       <c r="M3" s="10"/>
     </row>
-    <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8">
         <v>43839</v>
       </c>
@@ -870,7 +870,7 @@
       </c>
       <c r="M4" s="10"/>
     </row>
-    <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
         <v>43839</v>
       </c>
@@ -909,7 +909,7 @@
       </c>
       <c r="M5" s="10"/>
     </row>
-    <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8">
         <v>43843</v>
       </c>
@@ -948,7 +948,7 @@
       </c>
       <c r="M6" s="10"/>
     </row>
-    <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
         <v>43843</v>
       </c>
@@ -987,7 +987,7 @@
       </c>
       <c r="M7" s="10"/>
     </row>
-    <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
         <v>43843</v>
       </c>
@@ -1026,7 +1026,7 @@
       </c>
       <c r="M8" s="10"/>
     </row>
-    <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
         <v>43844</v>
       </c>
@@ -1065,7 +1065,7 @@
       </c>
       <c r="M9" s="10"/>
     </row>
-    <row r="10" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="8">
         <v>43844</v>
       </c>
@@ -1104,7 +1104,7 @@
       </c>
       <c r="M10" s="10"/>
     </row>
-    <row r="11" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="8">
         <v>43852</v>
       </c>
@@ -1143,7 +1143,7 @@
       </c>
       <c r="M11" s="10"/>
     </row>
-    <row r="12" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="8">
         <v>43852</v>
       </c>
@@ -1182,7 +1182,7 @@
       </c>
       <c r="M12" s="10"/>
     </row>
-    <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="8">
         <v>43852</v>
       </c>
@@ -1221,7 +1221,7 @@
       </c>
       <c r="M13" s="10"/>
     </row>
-    <row r="14" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="8">
         <v>43852</v>
       </c>
@@ -1260,7 +1260,7 @@
       </c>
       <c r="M14" s="10"/>
     </row>
-    <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="8">
         <v>43854</v>
       </c>
@@ -1299,7 +1299,7 @@
       </c>
       <c r="M15" s="10"/>
     </row>
-    <row r="16" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8">
         <v>43854</v>
       </c>
@@ -1338,7 +1338,7 @@
       </c>
       <c r="M16" s="10"/>
     </row>
-    <row r="17" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="8">
         <v>43854</v>
       </c>
@@ -1377,7 +1377,7 @@
       </c>
       <c r="M17" s="10"/>
     </row>
-    <row r="18" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="12"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -1392,7 +1392,7 @@
       <c r="L18" s="5"/>
       <c r="M18" s="2"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="12"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -1407,7 +1407,7 @@
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -1422,7 +1422,7 @@
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -1436,7 +1436,7 @@
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -1450,7 +1450,7 @@
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -1464,7 +1464,7 @@
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -1478,7 +1478,7 @@
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -1492,7 +1492,7 @@
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -1506,7 +1506,7 @@
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -1520,7 +1520,7 @@
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -1534,7 +1534,7 @@
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -1548,7 +1548,7 @@
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -1562,7 +1562,7 @@
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -1576,7 +1576,7 @@
       <c r="K31" s="2"/>
       <c r="L31" s="2"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -1590,7 +1590,7 @@
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -1604,7 +1604,7 @@
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -1618,7 +1618,7 @@
       <c r="K34" s="2"/>
       <c r="L34" s="2"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -1632,7 +1632,7 @@
       <c r="K35" s="2"/>
       <c r="L35" s="2"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -1646,7 +1646,7 @@
       <c r="K36" s="2"/>
       <c r="L36" s="2"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -1660,7 +1660,7 @@
       <c r="K37" s="2"/>
       <c r="L37" s="2"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -1674,7 +1674,7 @@
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -1688,7 +1688,7 @@
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -1702,7 +1702,7 @@
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -1716,7 +1716,7 @@
       <c r="K41" s="2"/>
       <c r="L41" s="2"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -1730,7 +1730,7 @@
       <c r="K42" s="2"/>
       <c r="L42" s="2"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -1744,7 +1744,7 @@
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -1758,7 +1758,7 @@
       <c r="K44" s="2"/>
       <c r="L44" s="2"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -1772,7 +1772,7 @@
       <c r="K45" s="2"/>
       <c r="L45" s="2"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -1786,7 +1786,7 @@
       <c r="K46" s="2"/>
       <c r="L46" s="2"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -1800,7 +1800,7 @@
       <c r="K47" s="2"/>
       <c r="L47" s="2"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -1814,7 +1814,7 @@
       <c r="K48" s="2"/>
       <c r="L48" s="2"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -1828,7 +1828,7 @@
       <c r="K49" s="2"/>
       <c r="L49" s="2"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
@@ -1842,7 +1842,7 @@
       <c r="K50" s="2"/>
       <c r="L50" s="2"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
@@ -1856,7 +1856,7 @@
       <c r="K51" s="2"/>
       <c r="L51" s="2"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
@@ -1870,7 +1870,7 @@
       <c r="K52" s="2"/>
       <c r="L52" s="2"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
@@ -1884,7 +1884,7 @@
       <c r="K53" s="2"/>
       <c r="L53" s="2"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
@@ -1898,7 +1898,7 @@
       <c r="K54" s="2"/>
       <c r="L54" s="2"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
@@ -1912,7 +1912,7 @@
       <c r="K55" s="2"/>
       <c r="L55" s="2"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
@@ -1926,7 +1926,7 @@
       <c r="K56" s="2"/>
       <c r="L56" s="2"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
@@ -1940,7 +1940,7 @@
       <c r="K57" s="2"/>
       <c r="L57" s="2"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
@@ -1954,7 +1954,7 @@
       <c r="K58" s="2"/>
       <c r="L58" s="2"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
@@ -1968,7 +1968,7 @@
       <c r="K59" s="2"/>
       <c r="L59" s="2"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
@@ -1982,7 +1982,7 @@
       <c r="K60" s="2"/>
       <c r="L60" s="2"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
@@ -1996,7 +1996,7 @@
       <c r="K61" s="2"/>
       <c r="L61" s="2"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
@@ -2010,7 +2010,7 @@
       <c r="K62" s="2"/>
       <c r="L62" s="2"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
@@ -2024,7 +2024,7 @@
       <c r="K63" s="2"/>
       <c r="L63" s="2"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
@@ -2038,7 +2038,7 @@
       <c r="K64" s="2"/>
       <c r="L64" s="2"/>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
@@ -2052,7 +2052,7 @@
       <c r="K65" s="2"/>
       <c r="L65" s="2"/>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
@@ -2066,7 +2066,7 @@
       <c r="K66" s="2"/>
       <c r="L66" s="2"/>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
@@ -2080,7 +2080,7 @@
       <c r="K67" s="2"/>
       <c r="L67" s="2"/>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
@@ -2094,7 +2094,7 @@
       <c r="K68" s="2"/>
       <c r="L68" s="2"/>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
@@ -2108,7 +2108,7 @@
       <c r="K69" s="2"/>
       <c r="L69" s="2"/>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A70" s="2"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
@@ -2122,7 +2122,7 @@
       <c r="K70" s="2"/>
       <c r="L70" s="2"/>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
@@ -2136,7 +2136,7 @@
       <c r="K71" s="2"/>
       <c r="L71" s="2"/>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
@@ -2150,7 +2150,7 @@
       <c r="K72" s="2"/>
       <c r="L72" s="2"/>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
@@ -2164,7 +2164,7 @@
       <c r="K73" s="2"/>
       <c r="L73" s="2"/>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
@@ -2178,7 +2178,7 @@
       <c r="K74" s="2"/>
       <c r="L74" s="2"/>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
@@ -2192,7 +2192,7 @@
       <c r="K75" s="2"/>
       <c r="L75" s="2"/>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
@@ -2206,7 +2206,7 @@
       <c r="K76" s="2"/>
       <c r="L76" s="2"/>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A77" s="2"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
@@ -2220,7 +2220,7 @@
       <c r="K77" s="2"/>
       <c r="L77" s="2"/>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A78" s="2"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
@@ -2234,7 +2234,7 @@
       <c r="K78" s="2"/>
       <c r="L78" s="2"/>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A79" s="2"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
@@ -2248,7 +2248,7 @@
       <c r="K79" s="2"/>
       <c r="L79" s="2"/>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A80" s="2"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
@@ -2262,7 +2262,7 @@
       <c r="K80" s="2"/>
       <c r="L80" s="2"/>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A81" s="2"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
@@ -2276,7 +2276,7 @@
       <c r="K81" s="2"/>
       <c r="L81" s="2"/>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
@@ -2290,7 +2290,7 @@
       <c r="K82" s="2"/>
       <c r="L82" s="2"/>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
@@ -2304,7 +2304,7 @@
       <c r="K83" s="2"/>
       <c r="L83" s="2"/>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A84" s="2"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
@@ -2318,7 +2318,7 @@
       <c r="K84" s="2"/>
       <c r="L84" s="2"/>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A85" s="2"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
@@ -2332,7 +2332,7 @@
       <c r="K85" s="2"/>
       <c r="L85" s="2"/>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A86" s="2"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
@@ -2346,7 +2346,7 @@
       <c r="K86" s="2"/>
       <c r="L86" s="2"/>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A87" s="2"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
@@ -2360,7 +2360,7 @@
       <c r="K87" s="2"/>
       <c r="L87" s="2"/>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A88" s="2"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
@@ -2374,7 +2374,7 @@
       <c r="K88" s="2"/>
       <c r="L88" s="2"/>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A89" s="2"/>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
@@ -2388,7 +2388,7 @@
       <c r="K89" s="2"/>
       <c r="L89" s="2"/>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A90" s="2"/>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
@@ -2402,7 +2402,7 @@
       <c r="K90" s="2"/>
       <c r="L90" s="2"/>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A91" s="2"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
@@ -2416,7 +2416,7 @@
       <c r="K91" s="2"/>
       <c r="L91" s="2"/>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A92" s="2"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
@@ -2430,7 +2430,7 @@
       <c r="K92" s="2"/>
       <c r="L92" s="2"/>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A93" s="2"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
@@ -2444,7 +2444,7 @@
       <c r="K93" s="2"/>
       <c r="L93" s="2"/>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A94" s="2"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
@@ -2458,7 +2458,7 @@
       <c r="K94" s="2"/>
       <c r="L94" s="2"/>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A95" s="2"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
@@ -2472,7 +2472,7 @@
       <c r="K95" s="2"/>
       <c r="L95" s="2"/>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A96" s="2"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
@@ -2486,7 +2486,7 @@
       <c r="K96" s="2"/>
       <c r="L96" s="2"/>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A97" s="2"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
@@ -2500,7 +2500,7 @@
       <c r="K97" s="2"/>
       <c r="L97" s="2"/>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A98" s="2"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
@@ -2514,7 +2514,7 @@
       <c r="K98" s="2"/>
       <c r="L98" s="2"/>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A99" s="2"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
@@ -2528,7 +2528,7 @@
       <c r="K99" s="2"/>
       <c r="L99" s="2"/>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A100" s="2"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
@@ -2542,7 +2542,7 @@
       <c r="K100" s="2"/>
       <c r="L100" s="2"/>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A101" s="2"/>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
@@ -2556,7 +2556,7 @@
       <c r="K101" s="2"/>
       <c r="L101" s="2"/>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A102" s="2"/>
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
@@ -2570,7 +2570,7 @@
       <c r="K102" s="2"/>
       <c r="L102" s="2"/>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A103" s="2"/>
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
@@ -2584,7 +2584,7 @@
       <c r="K103" s="2"/>
       <c r="L103" s="2"/>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A104" s="2"/>
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
@@ -2598,7 +2598,7 @@
       <c r="K104" s="2"/>
       <c r="L104" s="2"/>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A105" s="2"/>
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
@@ -2612,7 +2612,7 @@
       <c r="K105" s="2"/>
       <c r="L105" s="2"/>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A106" s="2"/>
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
@@ -2626,7 +2626,7 @@
       <c r="K106" s="2"/>
       <c r="L106" s="2"/>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A107" s="2"/>
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
@@ -2640,7 +2640,7 @@
       <c r="K107" s="2"/>
       <c r="L107" s="2"/>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A108" s="2"/>
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
@@ -2654,7 +2654,7 @@
       <c r="K108" s="2"/>
       <c r="L108" s="2"/>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A109" s="2"/>
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
@@ -2668,7 +2668,7 @@
       <c r="K109" s="2"/>
       <c r="L109" s="2"/>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A110" s="2"/>
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
@@ -2682,7 +2682,7 @@
       <c r="K110" s="2"/>
       <c r="L110" s="2"/>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A111" s="2"/>
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
@@ -2696,7 +2696,7 @@
       <c r="K111" s="2"/>
       <c r="L111" s="2"/>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A112" s="2"/>
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
@@ -2710,7 +2710,7 @@
       <c r="K112" s="2"/>
       <c r="L112" s="2"/>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A113" s="2"/>
       <c r="B113" s="2"/>
       <c r="C113" s="2"/>
@@ -2724,7 +2724,7 @@
       <c r="K113" s="2"/>
       <c r="L113" s="2"/>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A114" s="2"/>
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
@@ -2738,7 +2738,7 @@
       <c r="K114" s="2"/>
       <c r="L114" s="2"/>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A115" s="2"/>
       <c r="B115" s="2"/>
       <c r="C115" s="2"/>
@@ -2752,7 +2752,7 @@
       <c r="K115" s="2"/>
       <c r="L115" s="2"/>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A116" s="2"/>
       <c r="B116" s="2"/>
       <c r="C116" s="2"/>
@@ -2766,7 +2766,7 @@
       <c r="K116" s="2"/>
       <c r="L116" s="2"/>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A117" s="2"/>
       <c r="B117" s="2"/>
       <c r="C117" s="2"/>
@@ -2780,7 +2780,7 @@
       <c r="K117" s="2"/>
       <c r="L117" s="2"/>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A118" s="2"/>
       <c r="B118" s="2"/>
       <c r="C118" s="2"/>
@@ -2794,7 +2794,7 @@
       <c r="K118" s="2"/>
       <c r="L118" s="2"/>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A119" s="2"/>
       <c r="B119" s="2"/>
       <c r="C119" s="2"/>
@@ -2808,7 +2808,7 @@
       <c r="K119" s="2"/>
       <c r="L119" s="2"/>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A120" s="2"/>
       <c r="B120" s="2"/>
       <c r="C120" s="2"/>

</xml_diff>

<commit_message>
added dummy folders and dummy files to the justification evidence folder. Also changed values in the evidence location column of the findings tracker to lead to FOLDER/Mainfolder/...
</commit_message>
<xml_diff>
--- a/FOLDER/Mainfolder/Daily_Change_Monitoring/Findings Tracker.xlsx
+++ b/FOLDER/Mainfolder/Daily_Change_Monitoring/Findings Tracker.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1551b3744a113d45/Documents/UiPath/Robotic_Process_Automation/FOLDER/Mainfolder/Daily_Change_Monitoring/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S\Documents\UiPath_2\Robotic_Process_Automation\FOLDER\Mainfolder\Daily_Change_Monitoring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="114_{8AB96BB5-B659-4EAD-A8B6-E1AFCAECE06F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3356987-FA79-4768-B06A-9D3792DE5B95}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4008" yWindow="2256" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FindingsTracker" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="98">
   <si>
     <t>Date of Delta</t>
   </si>
@@ -282,33 +282,6 @@
     <t>CHR0000192847.pdf</t>
   </si>
   <si>
-    <t>\\MainFolder\Remediation_or_Justification Evidence\1-09-2020\RE: Random Email.msg</t>
-  </si>
-  <si>
-    <t>\\MainFolder\Remediation_or_Justification Evidence\1-22-2020\RE: Random Email.msg</t>
-  </si>
-  <si>
-    <t>\\MainFolder\Remediation_or_Justification Evidence\1-24-2020\RE: Random Email.msg</t>
-  </si>
-  <si>
-    <t>\\MainFolder\Remediation_or_Justification Evidence\1-09-2020\CHR0000928476.pdf</t>
-  </si>
-  <si>
-    <t>\\MainFolder\Remediation_or_Justification Evidence\1-22-2020\CHR0000391114.pdf</t>
-  </si>
-  <si>
-    <t>\\MainFolder\Remediation_or_Justification Evidence\1-24-2020\CHR0000381057.pdf</t>
-  </si>
-  <si>
-    <t>\\MainFolder\Remediation_or_Justification Evidence\1-24-2020\CHR0000382957.pdf</t>
-  </si>
-  <si>
-    <t>\\MainFolder\Remediation_or_Justification Evidence\1-09-2020\RandomFolder1\</t>
-  </si>
-  <si>
-    <t>\\MainFolder\Remediation_or_Justification Evidence\1-22-2020\RandomFolder2\</t>
-  </si>
-  <si>
     <t>FOLDER\Mainfolder\Remediation_or_Justification Evidence\1-09-2020\RE: Random Email.msg</t>
   </si>
   <si>
@@ -322,6 +295,30 @@
   </si>
   <si>
     <t>FOLDER\Mainfolder\Remediation_or_Justification Evidence\1-14-2020\CHR0000291924.pdf</t>
+  </si>
+  <si>
+    <t>FOLDER\Mainfolder\Remediation_or_Justification Evidence\1-09-2020\RandomFolder1\</t>
+  </si>
+  <si>
+    <t>FOLDER\Mainfolder\Remediation_or_Justification Evidence\1-09-2020\CHR0000928476.pdf</t>
+  </si>
+  <si>
+    <t>FOLDER\Mainfolder\Remediation_or_Justification Evidence\1-22-2020\RandomFolder2\</t>
+  </si>
+  <si>
+    <t>FOLDER\Mainfolder\Remediation_or_Justification Evidence\1-22-2020\CHR0000391114.pdf</t>
+  </si>
+  <si>
+    <t>FOLDER\Mainfolder\Remediation_or_Justification Evidence\1-22-2020\RE: Random Email.msg</t>
+  </si>
+  <si>
+    <t>FOLDER\Mainfolder\Remediation_or_Justification Evidence\1-24-2020\CHR0000381057.pdf</t>
+  </si>
+  <si>
+    <t>FOLDER\Mainfolder\Remediation_or_Justification Evidence\1-24-2020\CHR0000382957.pdf</t>
+  </si>
+  <si>
+    <t>FOLDER\Mainfolder\Remediation_or_Justification Evidence\1-24-2020\RE: Random Email.msg</t>
   </si>
 </sst>
 </file>
@@ -691,28 +688,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2:M17"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" customWidth="1"/>
+    <col min="1" max="1" width="11.6328125" customWidth="1"/>
+    <col min="2" max="2" width="15.36328125" customWidth="1"/>
+    <col min="3" max="3" width="15.453125" customWidth="1"/>
     <col min="4" max="4" width="61" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.33203125" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" customWidth="1"/>
-    <col min="7" max="7" width="18.44140625" customWidth="1"/>
+    <col min="5" max="5" width="21.36328125" customWidth="1"/>
+    <col min="6" max="6" width="17.6328125" customWidth="1"/>
+    <col min="7" max="7" width="18.453125" customWidth="1"/>
     <col min="8" max="8" width="22" customWidth="1"/>
-    <col min="9" max="9" width="21.44140625" customWidth="1"/>
+    <col min="9" max="9" width="21.453125" customWidth="1"/>
     <col min="10" max="10" width="11" customWidth="1"/>
     <col min="11" max="11" width="29" customWidth="1"/>
-    <col min="12" max="12" width="92.44140625" customWidth="1"/>
+    <col min="12" max="12" width="92.453125" customWidth="1"/>
     <col min="13" max="13" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="54" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="55.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -753,7 +750,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8">
         <v>43839</v>
       </c>
@@ -792,7 +789,7 @@
       </c>
       <c r="M2" s="10"/>
     </row>
-    <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="8">
         <v>43839</v>
       </c>
@@ -831,7 +828,7 @@
       </c>
       <c r="M3" s="10"/>
     </row>
-    <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="8">
         <v>43839</v>
       </c>
@@ -866,11 +863,11 @@
         <v>84</v>
       </c>
       <c r="L4" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="M4" s="10"/>
     </row>
-    <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="8">
         <v>43839</v>
       </c>
@@ -905,11 +902,11 @@
         <v>83</v>
       </c>
       <c r="L5" s="7" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="M5" s="10"/>
     </row>
-    <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="8">
         <v>43843</v>
       </c>
@@ -944,11 +941,11 @@
         <v>75</v>
       </c>
       <c r="L6" s="7" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="M6" s="10"/>
     </row>
-    <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="8">
         <v>43843</v>
       </c>
@@ -983,11 +980,11 @@
         <v>82</v>
       </c>
       <c r="L7" s="7" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="M7" s="10"/>
     </row>
-    <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="8">
         <v>43843</v>
       </c>
@@ -1022,11 +1019,11 @@
         <v>81</v>
       </c>
       <c r="L8" s="7" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="M8" s="10"/>
     </row>
-    <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="8">
         <v>43844</v>
       </c>
@@ -1061,11 +1058,11 @@
         <v>75</v>
       </c>
       <c r="L9" s="7" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="M9" s="10"/>
     </row>
-    <row r="10" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="8">
         <v>43844</v>
       </c>
@@ -1100,11 +1097,11 @@
         <v>80</v>
       </c>
       <c r="L10" s="7" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="M10" s="10"/>
     </row>
-    <row r="11" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="8">
         <v>43852</v>
       </c>
@@ -1139,11 +1136,11 @@
         <v>79</v>
       </c>
       <c r="L11" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="M11" s="10"/>
     </row>
-    <row r="12" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="8">
         <v>43852</v>
       </c>
@@ -1178,11 +1175,11 @@
         <v>78</v>
       </c>
       <c r="L12" s="7" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="M12" s="10"/>
     </row>
-    <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="8">
         <v>43852</v>
       </c>
@@ -1217,11 +1214,11 @@
         <v>75</v>
       </c>
       <c r="L13" s="7" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="M13" s="10"/>
     </row>
-    <row r="14" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="8">
         <v>43852</v>
       </c>
@@ -1256,11 +1253,11 @@
         <v>75</v>
       </c>
       <c r="L14" s="7" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="M14" s="10"/>
     </row>
-    <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="8">
         <v>43854</v>
       </c>
@@ -1295,11 +1292,11 @@
         <v>77</v>
       </c>
       <c r="L15" s="7" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="M15" s="10"/>
     </row>
-    <row r="16" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="8">
         <v>43854</v>
       </c>
@@ -1334,11 +1331,11 @@
         <v>76</v>
       </c>
       <c r="L16" s="7" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="M16" s="10"/>
     </row>
-    <row r="17" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="8">
         <v>43854</v>
       </c>
@@ -1373,11 +1370,11 @@
         <v>75</v>
       </c>
       <c r="L17" s="7" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="M17" s="10"/>
     </row>
-    <row r="18" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="12"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -1392,7 +1389,7 @@
       <c r="L18" s="5"/>
       <c r="M18" s="2"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="12"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -1407,7 +1404,7 @@
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -1422,7 +1419,7 @@
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -1436,7 +1433,7 @@
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -1450,7 +1447,7 @@
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -1464,7 +1461,7 @@
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -1478,7 +1475,7 @@
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -1492,7 +1489,7 @@
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -1506,7 +1503,7 @@
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -1520,7 +1517,7 @@
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -1534,7 +1531,7 @@
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -1548,7 +1545,7 @@
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -1562,7 +1559,7 @@
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -1576,7 +1573,7 @@
       <c r="K31" s="2"/>
       <c r="L31" s="2"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -1590,7 +1587,7 @@
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -1604,7 +1601,7 @@
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -1618,7 +1615,7 @@
       <c r="K34" s="2"/>
       <c r="L34" s="2"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -1632,7 +1629,7 @@
       <c r="K35" s="2"/>
       <c r="L35" s="2"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -1646,7 +1643,7 @@
       <c r="K36" s="2"/>
       <c r="L36" s="2"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -1660,7 +1657,7 @@
       <c r="K37" s="2"/>
       <c r="L37" s="2"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -1674,7 +1671,7 @@
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -1688,7 +1685,7 @@
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -1702,7 +1699,7 @@
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -1716,7 +1713,7 @@
       <c r="K41" s="2"/>
       <c r="L41" s="2"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -1730,7 +1727,7 @@
       <c r="K42" s="2"/>
       <c r="L42" s="2"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -1744,7 +1741,7 @@
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -1758,7 +1755,7 @@
       <c r="K44" s="2"/>
       <c r="L44" s="2"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -1772,7 +1769,7 @@
       <c r="K45" s="2"/>
       <c r="L45" s="2"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -1786,7 +1783,7 @@
       <c r="K46" s="2"/>
       <c r="L46" s="2"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -1800,7 +1797,7 @@
       <c r="K47" s="2"/>
       <c r="L47" s="2"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -1814,7 +1811,7 @@
       <c r="K48" s="2"/>
       <c r="L48" s="2"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -1828,7 +1825,7 @@
       <c r="K49" s="2"/>
       <c r="L49" s="2"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
@@ -1842,7 +1839,7 @@
       <c r="K50" s="2"/>
       <c r="L50" s="2"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
@@ -1856,7 +1853,7 @@
       <c r="K51" s="2"/>
       <c r="L51" s="2"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
@@ -1870,7 +1867,7 @@
       <c r="K52" s="2"/>
       <c r="L52" s="2"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
@@ -1884,7 +1881,7 @@
       <c r="K53" s="2"/>
       <c r="L53" s="2"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
@@ -1898,7 +1895,7 @@
       <c r="K54" s="2"/>
       <c r="L54" s="2"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
@@ -1912,7 +1909,7 @@
       <c r="K55" s="2"/>
       <c r="L55" s="2"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
@@ -1926,7 +1923,7 @@
       <c r="K56" s="2"/>
       <c r="L56" s="2"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
@@ -1940,7 +1937,7 @@
       <c r="K57" s="2"/>
       <c r="L57" s="2"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
@@ -1954,7 +1951,7 @@
       <c r="K58" s="2"/>
       <c r="L58" s="2"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
@@ -1968,7 +1965,7 @@
       <c r="K59" s="2"/>
       <c r="L59" s="2"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
@@ -1982,7 +1979,7 @@
       <c r="K60" s="2"/>
       <c r="L60" s="2"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
@@ -1996,7 +1993,7 @@
       <c r="K61" s="2"/>
       <c r="L61" s="2"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
@@ -2010,7 +2007,7 @@
       <c r="K62" s="2"/>
       <c r="L62" s="2"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
@@ -2024,7 +2021,7 @@
       <c r="K63" s="2"/>
       <c r="L63" s="2"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
@@ -2038,7 +2035,7 @@
       <c r="K64" s="2"/>
       <c r="L64" s="2"/>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
@@ -2052,7 +2049,7 @@
       <c r="K65" s="2"/>
       <c r="L65" s="2"/>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
@@ -2066,7 +2063,7 @@
       <c r="K66" s="2"/>
       <c r="L66" s="2"/>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
@@ -2080,7 +2077,7 @@
       <c r="K67" s="2"/>
       <c r="L67" s="2"/>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
@@ -2094,7 +2091,7 @@
       <c r="K68" s="2"/>
       <c r="L68" s="2"/>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
@@ -2108,7 +2105,7 @@
       <c r="K69" s="2"/>
       <c r="L69" s="2"/>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A70" s="2"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
@@ -2122,7 +2119,7 @@
       <c r="K70" s="2"/>
       <c r="L70" s="2"/>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
@@ -2136,7 +2133,7 @@
       <c r="K71" s="2"/>
       <c r="L71" s="2"/>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
@@ -2150,7 +2147,7 @@
       <c r="K72" s="2"/>
       <c r="L72" s="2"/>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
@@ -2164,7 +2161,7 @@
       <c r="K73" s="2"/>
       <c r="L73" s="2"/>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
@@ -2178,7 +2175,7 @@
       <c r="K74" s="2"/>
       <c r="L74" s="2"/>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
@@ -2192,7 +2189,7 @@
       <c r="K75" s="2"/>
       <c r="L75" s="2"/>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
@@ -2206,7 +2203,7 @@
       <c r="K76" s="2"/>
       <c r="L76" s="2"/>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A77" s="2"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
@@ -2220,7 +2217,7 @@
       <c r="K77" s="2"/>
       <c r="L77" s="2"/>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A78" s="2"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
@@ -2234,7 +2231,7 @@
       <c r="K78" s="2"/>
       <c r="L78" s="2"/>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A79" s="2"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
@@ -2248,7 +2245,7 @@
       <c r="K79" s="2"/>
       <c r="L79" s="2"/>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A80" s="2"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
@@ -2262,7 +2259,7 @@
       <c r="K80" s="2"/>
       <c r="L80" s="2"/>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A81" s="2"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
@@ -2276,7 +2273,7 @@
       <c r="K81" s="2"/>
       <c r="L81" s="2"/>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
@@ -2290,7 +2287,7 @@
       <c r="K82" s="2"/>
       <c r="L82" s="2"/>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
@@ -2304,7 +2301,7 @@
       <c r="K83" s="2"/>
       <c r="L83" s="2"/>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A84" s="2"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
@@ -2318,7 +2315,7 @@
       <c r="K84" s="2"/>
       <c r="L84" s="2"/>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A85" s="2"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
@@ -2332,7 +2329,7 @@
       <c r="K85" s="2"/>
       <c r="L85" s="2"/>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A86" s="2"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
@@ -2346,7 +2343,7 @@
       <c r="K86" s="2"/>
       <c r="L86" s="2"/>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A87" s="2"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
@@ -2360,7 +2357,7 @@
       <c r="K87" s="2"/>
       <c r="L87" s="2"/>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A88" s="2"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
@@ -2374,7 +2371,7 @@
       <c r="K88" s="2"/>
       <c r="L88" s="2"/>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A89" s="2"/>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
@@ -2388,7 +2385,7 @@
       <c r="K89" s="2"/>
       <c r="L89" s="2"/>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A90" s="2"/>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
@@ -2402,7 +2399,7 @@
       <c r="K90" s="2"/>
       <c r="L90" s="2"/>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A91" s="2"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
@@ -2416,7 +2413,7 @@
       <c r="K91" s="2"/>
       <c r="L91" s="2"/>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A92" s="2"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
@@ -2430,7 +2427,7 @@
       <c r="K92" s="2"/>
       <c r="L92" s="2"/>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A93" s="2"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
@@ -2444,7 +2441,7 @@
       <c r="K93" s="2"/>
       <c r="L93" s="2"/>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A94" s="2"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
@@ -2458,7 +2455,7 @@
       <c r="K94" s="2"/>
       <c r="L94" s="2"/>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A95" s="2"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
@@ -2472,7 +2469,7 @@
       <c r="K95" s="2"/>
       <c r="L95" s="2"/>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A96" s="2"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
@@ -2486,7 +2483,7 @@
       <c r="K96" s="2"/>
       <c r="L96" s="2"/>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A97" s="2"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
@@ -2500,7 +2497,7 @@
       <c r="K97" s="2"/>
       <c r="L97" s="2"/>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A98" s="2"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
@@ -2514,7 +2511,7 @@
       <c r="K98" s="2"/>
       <c r="L98" s="2"/>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A99" s="2"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
@@ -2528,7 +2525,7 @@
       <c r="K99" s="2"/>
       <c r="L99" s="2"/>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A100" s="2"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
@@ -2542,7 +2539,7 @@
       <c r="K100" s="2"/>
       <c r="L100" s="2"/>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A101" s="2"/>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
@@ -2556,7 +2553,7 @@
       <c r="K101" s="2"/>
       <c r="L101" s="2"/>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A102" s="2"/>
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
@@ -2570,7 +2567,7 @@
       <c r="K102" s="2"/>
       <c r="L102" s="2"/>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A103" s="2"/>
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
@@ -2584,7 +2581,7 @@
       <c r="K103" s="2"/>
       <c r="L103" s="2"/>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A104" s="2"/>
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
@@ -2598,7 +2595,7 @@
       <c r="K104" s="2"/>
       <c r="L104" s="2"/>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A105" s="2"/>
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
@@ -2612,7 +2609,7 @@
       <c r="K105" s="2"/>
       <c r="L105" s="2"/>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A106" s="2"/>
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
@@ -2626,7 +2623,7 @@
       <c r="K106" s="2"/>
       <c r="L106" s="2"/>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A107" s="2"/>
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
@@ -2640,7 +2637,7 @@
       <c r="K107" s="2"/>
       <c r="L107" s="2"/>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A108" s="2"/>
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
@@ -2654,7 +2651,7 @@
       <c r="K108" s="2"/>
       <c r="L108" s="2"/>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A109" s="2"/>
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
@@ -2668,7 +2665,7 @@
       <c r="K109" s="2"/>
       <c r="L109" s="2"/>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A110" s="2"/>
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
@@ -2682,7 +2679,7 @@
       <c r="K110" s="2"/>
       <c r="L110" s="2"/>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A111" s="2"/>
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
@@ -2696,7 +2693,7 @@
       <c r="K111" s="2"/>
       <c r="L111" s="2"/>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A112" s="2"/>
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
@@ -2710,7 +2707,7 @@
       <c r="K112" s="2"/>
       <c r="L112" s="2"/>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A113" s="2"/>
       <c r="B113" s="2"/>
       <c r="C113" s="2"/>
@@ -2724,7 +2721,7 @@
       <c r="K113" s="2"/>
       <c r="L113" s="2"/>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A114" s="2"/>
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
@@ -2738,7 +2735,7 @@
       <c r="K114" s="2"/>
       <c r="L114" s="2"/>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A115" s="2"/>
       <c r="B115" s="2"/>
       <c r="C115" s="2"/>
@@ -2752,7 +2749,7 @@
       <c r="K115" s="2"/>
       <c r="L115" s="2"/>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A116" s="2"/>
       <c r="B116" s="2"/>
       <c r="C116" s="2"/>
@@ -2766,7 +2763,7 @@
       <c r="K116" s="2"/>
       <c r="L116" s="2"/>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A117" s="2"/>
       <c r="B117" s="2"/>
       <c r="C117" s="2"/>
@@ -2780,7 +2777,7 @@
       <c r="K117" s="2"/>
       <c r="L117" s="2"/>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A118" s="2"/>
       <c r="B118" s="2"/>
       <c r="C118" s="2"/>
@@ -2794,7 +2791,7 @@
       <c r="K118" s="2"/>
       <c r="L118" s="2"/>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A119" s="2"/>
       <c r="B119" s="2"/>
       <c r="C119" s="2"/>
@@ -2808,7 +2805,7 @@
       <c r="K119" s="2"/>
       <c r="L119" s="2"/>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A120" s="2"/>
       <c r="B120" s="2"/>
       <c r="C120" s="2"/>
@@ -2842,24 +2839,24 @@
     <hyperlink ref="E12" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
     <hyperlink ref="E13" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
     <hyperlink ref="E14" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="L2" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="L2" r:id="rId19" display="\\MainFolder\Remediation_or_Justification Evidence\1-09-2020\RE: Random Email.msg" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
     <hyperlink ref="L6" r:id="rId20" display="\\MainFolder\Remediation_or_Justification Evidence\1-09-2020\RE: Random Email.msg" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
     <hyperlink ref="L9" r:id="rId21" display="\\MainFolder\Remediation_or_Justification Evidence\1-14-2020\RE: Random Email.msg" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="L14" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="L17" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="L13" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="L4" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="L5" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="L14" r:id="rId22" display="\\MainFolder\Remediation_or_Justification Evidence\1-22-2020\RE: Random Email.msg" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="L17" r:id="rId23" display="\\MainFolder\Remediation_or_Justification Evidence\1-24-2020\RE: Random Email.msg" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="L13" r:id="rId24" display="\\MainFolder\Remediation_or_Justification Evidence\1-22-2020\RE: Random Email.msg" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="L4" r:id="rId25" display="\\MainFolder\Remediation_or_Justification Evidence\1-09-2020\RandomFolder1\" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="L5" r:id="rId26" display="\\MainFolder\Remediation_or_Justification Evidence\1-09-2020\CHR0000928476.pdf" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
     <hyperlink ref="L7" r:id="rId27" display="\\MainFolder\Remediation_or_Justification Evidence\1-13-2020\CHR0000230943.pdf" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
     <hyperlink ref="L8" r:id="rId28" display="\\MainFolder\Remediation_or_Justification Evidence\1-13-2020\CHR0000123095.pdf" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
     <hyperlink ref="L10" r:id="rId29" display="\\MainFolder\Remediation_or_Justification Evidence\1-14-2020\CHR0000291924.pdf" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
     <hyperlink ref="L11:L12" r:id="rId30" display="\\MainFolder\Remediation_or_Justification Evidence\1-22-2020\RE: Random Email.msg" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="L11" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="L12" r:id="rId32" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="L11" r:id="rId31" display="\\MainFolder\Remediation_or_Justification Evidence\1-22-2020\RandomFolder2\" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="L12" r:id="rId32" display="\\MainFolder\Remediation_or_Justification Evidence\1-22-2020\CHR0000391114.pdf" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
     <hyperlink ref="L15:L16" r:id="rId33" display="\\MainFolder\Remediation_or_Justification Evidence\1-24-2020\RE: Random Email.msg" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="L15" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="L16" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="L3" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="L15" r:id="rId34" display="\\MainFolder\Remediation_or_Justification Evidence\1-24-2020\CHR0000381057.pdf" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="L16" r:id="rId35" display="\\MainFolder\Remediation_or_Justification Evidence\1-24-2020\CHR0000382957.pdf" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="L3" r:id="rId36" display="\\MainFolder\Remediation_or_Justification Evidence\1-09-2020\RE: Random Email.msg" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fixed formatting of section 3
</commit_message>
<xml_diff>
--- a/FOLDER/Mainfolder/Daily_Change_Monitoring/Findings Tracker.xlsx
+++ b/FOLDER/Mainfolder/Daily_Change_Monitoring/Findings Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S\Documents\UiPath_2\Robotic_Process_Automation\FOLDER\Mainfolder\Daily_Change_Monitoring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3356987-FA79-4768-B06A-9D3792DE5B95}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B3C15AC-9B2E-42D5-A026-8E28EDD7E868}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="93">
   <si>
     <t>Date of Delta</t>
   </si>
@@ -66,9 +66,6 @@
     <t>ITRCA Member that filed or reviewed(if BOT found) final evidence</t>
   </si>
   <si>
-    <t>magic_kl02</t>
-  </si>
-  <si>
     <t>magic_kq_023</t>
   </si>
   <si>
@@ -96,12 +93,6 @@
     <t>magic435</t>
   </si>
   <si>
-    <t>magic_qq_23455</t>
-  </si>
-  <si>
-    <t>test_2348q</t>
-  </si>
-  <si>
     <t>test234234</t>
   </si>
   <si>
@@ -141,12 +132,6 @@
     <t>CHANGES - SOX Audit Report for magic435.txt_07.01.73.eml</t>
   </si>
   <si>
-    <t>CHANGES - SOX Audit Report for magic_qq_23455.txt_07.01.73.eml</t>
-  </si>
-  <si>
-    <t>CHANGES - SOX Audit Report for test_2348q.txt_07.01.73.eml</t>
-  </si>
-  <si>
     <t>CHANGES - SOX Audit Report for test234234.txt_07.01.73.eml</t>
   </si>
   <si>
@@ -189,12 +174,6 @@
     <t>\\MainFolder\Daily_Change_Monitoring\1Jan2019\1-22-2020\CHANGES - SOX Audit Report for magic435.txt_07.01.73.eml</t>
   </si>
   <si>
-    <t>\\MainFolder\Daily_Change_Monitoring\1Jan2019\1-22-2020\CHANGES - SOX Audit Report for magic_qq_23455.txt_07.01.73.eml</t>
-  </si>
-  <si>
-    <t>\\MainFolder\Daily_Change_Monitoring\1Jan2019\1-22-2020\CHANGES - SOX Audit Report for test_2348q.txt_07.01.73.eml</t>
-  </si>
-  <si>
     <t>\\MainFolder\Daily_Change_Monitoring\1Jan2019\1-22-2020\CHANGES - SOX Audit Report for test234234.txt_07.01.73.eml</t>
   </si>
   <si>
@@ -228,9 +207,6 @@
     <t>CHR0000382957</t>
   </si>
   <si>
-    <t>CHR0000391114</t>
-  </si>
-  <si>
     <t>CHR0000295932</t>
   </si>
   <si>
@@ -240,9 +216,6 @@
     <t>CHR0000123095</t>
   </si>
   <si>
-    <t>CHR0000230943</t>
-  </si>
-  <si>
     <t>CHR0000192847</t>
   </si>
   <si>
@@ -261,9 +234,6 @@
     <t>CHR0000381057.pdf</t>
   </si>
   <si>
-    <t>CHR0000391114.pdf</t>
-  </si>
-  <si>
     <t>CHR0000295932.pdf</t>
   </si>
   <si>
@@ -294,9 +264,6 @@
     <t>FOLDER\Mainfolder\Remediation_or_Justification Evidence\1-14-2020\RE: Random Email.msg</t>
   </si>
   <si>
-    <t>FOLDER\Mainfolder\Remediation_or_Justification Evidence\1-14-2020\CHR0000291924.pdf</t>
-  </si>
-  <si>
     <t>FOLDER\Mainfolder\Remediation_or_Justification Evidence\1-09-2020\RandomFolder1\</t>
   </si>
   <si>
@@ -306,12 +273,6 @@
     <t>FOLDER\Mainfolder\Remediation_or_Justification Evidence\1-22-2020\RandomFolder2\</t>
   </si>
   <si>
-    <t>FOLDER\Mainfolder\Remediation_or_Justification Evidence\1-22-2020\CHR0000391114.pdf</t>
-  </si>
-  <si>
-    <t>FOLDER\Mainfolder\Remediation_or_Justification Evidence\1-22-2020\RE: Random Email.msg</t>
-  </si>
-  <si>
     <t>FOLDER\Mainfolder\Remediation_or_Justification Evidence\1-24-2020\CHR0000381057.pdf</t>
   </si>
   <si>
@@ -319,6 +280,30 @@
   </si>
   <si>
     <t>FOLDER\Mainfolder\Remediation_or_Justification Evidence\1-24-2020\RE: Random Email.msg</t>
+  </si>
+  <si>
+    <t>something</t>
+  </si>
+  <si>
+    <t>Invalid</t>
+  </si>
+  <si>
+    <t>CHANGES - MissingFromFolders oiuer3298.txt_07.01.73.eml</t>
+  </si>
+  <si>
+    <t>\\MainFolder\Daily_Change_Monitoring\1Jan2019\1-24-2020\CHANGES - MissingFromFolders oiuer3298.txt_07.01.73.eml</t>
+  </si>
+  <si>
+    <t>missing_server</t>
+  </si>
+  <si>
+    <t>RE: Random Email missing.msg</t>
+  </si>
+  <si>
+    <t>FOLDER\Mainfolder\Remediation_or_Justification Evidence\1-22-2020\RE: Random Email missing.msg</t>
+  </si>
+  <si>
+    <t>FOLDER\Mainfolder\Remediation_or_Justification Evidence\Invalid Folder\1-14-2020\CHR0000291924.pdf</t>
   </si>
 </sst>
 </file>
@@ -686,10 +671,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M120"/>
+  <dimension ref="A1:M118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -698,7 +683,7 @@
     <col min="2" max="2" width="15.36328125" customWidth="1"/>
     <col min="3" max="3" width="15.453125" customWidth="1"/>
     <col min="4" max="4" width="61" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.36328125" customWidth="1"/>
+    <col min="5" max="5" width="77.54296875" customWidth="1"/>
     <col min="6" max="6" width="17.6328125" customWidth="1"/>
     <col min="7" max="7" width="18.453125" customWidth="1"/>
     <col min="8" max="8" width="22" customWidth="1"/>
@@ -755,154 +740,160 @@
         <v>43839</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="K2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="L2" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="M2" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="M2" s="10"/>
     </row>
     <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="8">
         <v>43839</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="K3" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="L3" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="M3" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="M3" s="10"/>
     </row>
     <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="8">
         <v>43839</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="G4" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" s="10" t="s">
-        <v>72</v>
-      </c>
       <c r="J4" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="K4" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="K4" s="4" t="s">
-        <v>84</v>
-      </c>
       <c r="L4" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="M4" s="10"/>
+        <v>79</v>
+      </c>
+      <c r="M4" s="10" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="8">
         <v>43839</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I5" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="K5" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="J5" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>83</v>
-      </c>
       <c r="L5" s="7" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="M5" s="10"/>
     </row>
@@ -911,486 +902,484 @@
         <v>43843</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I6" s="10" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="K6" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="L6" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="L6" s="7" t="s">
+      <c r="M6" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="M6" s="10"/>
     </row>
     <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="8">
         <v>43843</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I7" s="10" t="s">
-        <v>71</v>
+        <v>86</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="L7" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="M7" s="10"/>
+        <v>76</v>
+      </c>
+      <c r="M7" s="10" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="8">
         <v>43843</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>13</v>
+        <v>89</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="L8" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="M8" s="10"/>
+        <v>77</v>
+      </c>
+      <c r="M8" s="10" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="8">
         <v>43844</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C9" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="H9" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>20</v>
-      </c>
       <c r="I9" s="10" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="L9" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="M9" s="10"/>
+        <v>78</v>
+      </c>
+      <c r="M9" s="10" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="10" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="8">
         <v>43844</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="L10" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="M10" s="10"/>
+        <v>92</v>
+      </c>
+      <c r="M10" s="10" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="11" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="8">
         <v>43852</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F11" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I11" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="G11" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I11" s="11" t="s">
-        <v>68</v>
-      </c>
       <c r="J11" s="10" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="L11" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="M11" s="10"/>
+        <v>81</v>
+      </c>
+      <c r="M11" s="10" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="12" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="8">
         <v>43852</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="I12" s="11" t="s">
-        <v>67</v>
+        <v>22</v>
+      </c>
+      <c r="I12" s="10" t="s">
+        <v>57</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="K12" s="5" t="s">
-        <v>78</v>
+        <v>65</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>90</v>
       </c>
       <c r="L12" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="M12" s="10"/>
+        <v>91</v>
+      </c>
+      <c r="M12" s="10" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="8">
-        <v>43852</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>61</v>
+        <v>43854</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>56</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I13" s="10" t="s">
-        <v>64</v>
+        <v>23</v>
+      </c>
+      <c r="I13" s="11" t="s">
+        <v>58</v>
       </c>
       <c r="J13" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="K13" s="4" t="s">
-        <v>75</v>
+        <v>65</v>
+      </c>
+      <c r="K13" s="5" t="s">
+        <v>68</v>
       </c>
       <c r="L13" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="M13" s="10"/>
+        <v>82</v>
+      </c>
+      <c r="M13" s="10" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="14" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="8">
-        <v>43852</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>61</v>
+        <v>43854</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="I14" s="10" t="s">
-        <v>64</v>
+        <v>24</v>
+      </c>
+      <c r="I14" s="11" t="s">
+        <v>59</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="K14" s="4" t="s">
-        <v>75</v>
+        <v>65</v>
+      </c>
+      <c r="K14" s="5" t="s">
+        <v>67</v>
       </c>
       <c r="L14" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="M14" s="10"/>
+        <v>83</v>
+      </c>
+      <c r="M14" s="10" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="8">
         <v>43854</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E15" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I15" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="F15" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="G15" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I15" s="11" t="s">
+      <c r="J15" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="J15" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="K15" s="5" t="s">
-        <v>77</v>
+      <c r="K15" s="4" t="s">
+        <v>66</v>
       </c>
       <c r="L15" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="M15" s="10"/>
+        <v>84</v>
+      </c>
+      <c r="M15" s="10" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="16" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="8">
         <v>43854</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>61</v>
+      <c r="B16" s="4" t="s">
+        <v>55</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>42</v>
+        <v>87</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>58</v>
+        <v>88</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="I16" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="I16" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="J16" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="K16" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="J16" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="K16" s="5" t="s">
-        <v>76</v>
-      </c>
       <c r="L16" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="M16" s="10"/>
-    </row>
-    <row r="17" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="8">
-        <v>43854</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="F17" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="G17" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="I17" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="J17" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="K17" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="L17" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="M17" s="10"/>
-    </row>
-    <row r="18" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="12"/>
+        <v>84</v>
+      </c>
+      <c r="M16" s="10" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A17" s="12"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
-      <c r="E18" s="5"/>
+      <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
-      <c r="L18" s="5"/>
+      <c r="L18" s="2"/>
       <c r="M18" s="2"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A19" s="12"/>
+      <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
@@ -1402,7 +1391,6 @@
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" s="2"/>
@@ -1417,7 +1405,6 @@
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" s="2"/>
@@ -2791,34 +2778,6 @@
       <c r="K118" s="2"/>
       <c r="L118" s="2"/>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A119" s="2"/>
-      <c r="B119" s="2"/>
-      <c r="C119" s="2"/>
-      <c r="D119" s="2"/>
-      <c r="E119" s="2"/>
-      <c r="F119" s="2"/>
-      <c r="G119" s="2"/>
-      <c r="H119" s="2"/>
-      <c r="I119" s="2"/>
-      <c r="J119" s="2"/>
-      <c r="K119" s="2"/>
-      <c r="L119" s="2"/>
-    </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A120" s="2"/>
-      <c r="B120" s="2"/>
-      <c r="C120" s="2"/>
-      <c r="D120" s="2"/>
-      <c r="E120" s="2"/>
-      <c r="F120" s="2"/>
-      <c r="G120" s="2"/>
-      <c r="H120" s="2"/>
-      <c r="I120" s="2"/>
-      <c r="J120" s="2"/>
-      <c r="K120" s="2"/>
-      <c r="L120" s="2"/>
-    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -2827,36 +2786,34 @@
     <hyperlink ref="E9" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
     <hyperlink ref="E10" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
     <hyperlink ref="E11" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="E12:E14" r:id="rId7" display="\\MainFolder\Daily_Change_Monitoring\1Jan2019\1-22-2020\" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="E16" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="E15" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="E17" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="E12" r:id="rId7" display="\\MainFolder\Daily_Change_Monitoring\1Jan2019\1-22-2020\" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="E14" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="E13" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="E15" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
     <hyperlink ref="E3" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
     <hyperlink ref="E4" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
     <hyperlink ref="E5" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
     <hyperlink ref="E7" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
     <hyperlink ref="E8" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="E12" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="E13" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="E14" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="L2" r:id="rId19" display="\\MainFolder\Remediation_or_Justification Evidence\1-09-2020\RE: Random Email.msg" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="L6" r:id="rId20" display="\\MainFolder\Remediation_or_Justification Evidence\1-09-2020\RE: Random Email.msg" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="L9" r:id="rId21" display="\\MainFolder\Remediation_or_Justification Evidence\1-14-2020\RE: Random Email.msg" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="L14" r:id="rId22" display="\\MainFolder\Remediation_or_Justification Evidence\1-22-2020\RE: Random Email.msg" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="L17" r:id="rId23" display="\\MainFolder\Remediation_or_Justification Evidence\1-24-2020\RE: Random Email.msg" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="L13" r:id="rId24" display="\\MainFolder\Remediation_or_Justification Evidence\1-22-2020\RE: Random Email.msg" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="L4" r:id="rId25" display="\\MainFolder\Remediation_or_Justification Evidence\1-09-2020\RandomFolder1\" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="L5" r:id="rId26" display="\\MainFolder\Remediation_or_Justification Evidence\1-09-2020\CHR0000928476.pdf" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="L7" r:id="rId27" display="\\MainFolder\Remediation_or_Justification Evidence\1-13-2020\CHR0000230943.pdf" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="L8" r:id="rId28" display="\\MainFolder\Remediation_or_Justification Evidence\1-13-2020\CHR0000123095.pdf" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="L10" r:id="rId29" display="\\MainFolder\Remediation_or_Justification Evidence\1-14-2020\CHR0000291924.pdf" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="L11:L12" r:id="rId30" display="\\MainFolder\Remediation_or_Justification Evidence\1-22-2020\RE: Random Email.msg" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="L11" r:id="rId31" display="\\MainFolder\Remediation_or_Justification Evidence\1-22-2020\RandomFolder2\" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="L12" r:id="rId32" display="\\MainFolder\Remediation_or_Justification Evidence\1-22-2020\CHR0000391114.pdf" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="L15:L16" r:id="rId33" display="\\MainFolder\Remediation_or_Justification Evidence\1-24-2020\RE: Random Email.msg" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="L15" r:id="rId34" display="\\MainFolder\Remediation_or_Justification Evidence\1-24-2020\CHR0000381057.pdf" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="L16" r:id="rId35" display="\\MainFolder\Remediation_or_Justification Evidence\1-24-2020\CHR0000382957.pdf" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="L3" r:id="rId36" display="\\MainFolder\Remediation_or_Justification Evidence\1-09-2020\RE: Random Email.msg" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="E12" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="L2" r:id="rId17" display="\\MainFolder\Remediation_or_Justification Evidence\1-09-2020\RE: Random Email.msg" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="L6" r:id="rId18" display="\\MainFolder\Remediation_or_Justification Evidence\1-09-2020\RE: Random Email.msg" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="L9" r:id="rId19" display="\\MainFolder\Remediation_or_Justification Evidence\1-14-2020\RE: Random Email.msg" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="L12" r:id="rId20" display="\\MainFolder\Remediation_or_Justification Evidence\1-22-2020\RE: Random Email.msg" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="L15" r:id="rId21" display="\\MainFolder\Remediation_or_Justification Evidence\1-24-2020\RE: Random Email.msg" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="L4" r:id="rId22" display="\\MainFolder\Remediation_or_Justification Evidence\1-09-2020\RandomFolder1\" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="L5" r:id="rId23" display="\\MainFolder\Remediation_or_Justification Evidence\1-09-2020\CHR0000928476.pdf" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="L7" r:id="rId24" display="\\MainFolder\Remediation_or_Justification Evidence\1-13-2020\CHR0000230943.pdf" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="L8" r:id="rId25" display="\\MainFolder\Remediation_or_Justification Evidence\1-13-2020\CHR0000123095.pdf" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="L10" r:id="rId26" display="\\MainFolder\Remediation_or_Justification Evidence\1-14-2020\CHR0000291924.pdf" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="L11" r:id="rId27" display="\\MainFolder\Remediation_or_Justification Evidence\1-22-2020\RE: Random Email.msg" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="L11" r:id="rId28" display="\\MainFolder\Remediation_or_Justification Evidence\1-22-2020\RandomFolder2\" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="L13:L14" r:id="rId29" display="\\MainFolder\Remediation_or_Justification Evidence\1-24-2020\RE: Random Email.msg" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="L13" r:id="rId30" display="\\MainFolder\Remediation_or_Justification Evidence\1-24-2020\CHR0000381057.pdf" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="L14" r:id="rId31" display="\\MainFolder\Remediation_or_Justification Evidence\1-24-2020\CHR0000382957.pdf" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="L3" r:id="rId32" display="\\MainFolder\Remediation_or_Justification Evidence\1-09-2020\RE: Random Email.msg" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="E16" r:id="rId33" xr:uid="{64586501-B352-4FCB-A33E-6BC1F8C98BC3}"/>
+    <hyperlink ref="L16" r:id="rId34" display="\\MainFolder\Remediation_or_Justification Evidence\1-24-2020\RE: Random Email.msg" xr:uid="{7AADC3FF-F4AF-4D4B-B372-93D0BBB254DF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
changes business exceptions and changed to alternate step 5 workflow
</commit_message>
<xml_diff>
--- a/FOLDER/Mainfolder/Daily_Change_Monitoring/Findings Tracker.xlsx
+++ b/FOLDER/Mainfolder/Daily_Change_Monitoring/Findings Tracker.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S\Documents\UiPath_2\Robotic_Process_Automation\FOLDER\Mainfolder\Daily_Change_Monitoring\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dylan\Documents\UiPath\Robotic_Process_Automation\FOLDER\Mainfolder\Daily_Change_Monitoring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3356987-FA79-4768-B06A-9D3792DE5B95}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01FACFA0-F1A8-47AF-ACBF-B45487FA8935}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FindingsTracker" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="93">
   <si>
     <t>Date of Delta</t>
   </si>
@@ -66,9 +66,6 @@
     <t>ITRCA Member that filed or reviewed(if BOT found) final evidence</t>
   </si>
   <si>
-    <t>magic_kl02</t>
-  </si>
-  <si>
     <t>magic_kq_023</t>
   </si>
   <si>
@@ -96,12 +93,6 @@
     <t>magic435</t>
   </si>
   <si>
-    <t>magic_qq_23455</t>
-  </si>
-  <si>
-    <t>test_2348q</t>
-  </si>
-  <si>
     <t>test234234</t>
   </si>
   <si>
@@ -141,12 +132,6 @@
     <t>CHANGES - SOX Audit Report for magic435.txt_07.01.73.eml</t>
   </si>
   <si>
-    <t>CHANGES - SOX Audit Report for magic_qq_23455.txt_07.01.73.eml</t>
-  </si>
-  <si>
-    <t>CHANGES - SOX Audit Report for test_2348q.txt_07.01.73.eml</t>
-  </si>
-  <si>
     <t>CHANGES - SOX Audit Report for test234234.txt_07.01.73.eml</t>
   </si>
   <si>
@@ -189,12 +174,6 @@
     <t>\\MainFolder\Daily_Change_Monitoring\1Jan2019\1-22-2020\CHANGES - SOX Audit Report for magic435.txt_07.01.73.eml</t>
   </si>
   <si>
-    <t>\\MainFolder\Daily_Change_Monitoring\1Jan2019\1-22-2020\CHANGES - SOX Audit Report for magic_qq_23455.txt_07.01.73.eml</t>
-  </si>
-  <si>
-    <t>\\MainFolder\Daily_Change_Monitoring\1Jan2019\1-22-2020\CHANGES - SOX Audit Report for test_2348q.txt_07.01.73.eml</t>
-  </si>
-  <si>
     <t>\\MainFolder\Daily_Change_Monitoring\1Jan2019\1-22-2020\CHANGES - SOX Audit Report for test234234.txt_07.01.73.eml</t>
   </si>
   <si>
@@ -228,9 +207,6 @@
     <t>CHR0000382957</t>
   </si>
   <si>
-    <t>CHR0000391114</t>
-  </si>
-  <si>
     <t>CHR0000295932</t>
   </si>
   <si>
@@ -240,9 +216,6 @@
     <t>CHR0000123095</t>
   </si>
   <si>
-    <t>CHR0000230943</t>
-  </si>
-  <si>
     <t>CHR0000192847</t>
   </si>
   <si>
@@ -261,9 +234,6 @@
     <t>CHR0000381057.pdf</t>
   </si>
   <si>
-    <t>CHR0000391114.pdf</t>
-  </si>
-  <si>
     <t>CHR0000295932.pdf</t>
   </si>
   <si>
@@ -282,21 +252,12 @@
     <t>CHR0000192847.pdf</t>
   </si>
   <si>
-    <t>FOLDER\Mainfolder\Remediation_or_Justification Evidence\1-09-2020\RE: Random Email.msg</t>
-  </si>
-  <si>
     <t>FOLDER\Mainfolder\Remediation_or_Justification Evidence\1-13-2020\CHR0000230943.pdf</t>
   </si>
   <si>
     <t>FOLDER\Mainfolder\Remediation_or_Justification Evidence\1-13-2020\</t>
   </si>
   <si>
-    <t>FOLDER\Mainfolder\Remediation_or_Justification Evidence\1-14-2020\RE: Random Email.msg</t>
-  </si>
-  <si>
-    <t>FOLDER\Mainfolder\Remediation_or_Justification Evidence\1-14-2020\CHR0000291924.pdf</t>
-  </si>
-  <si>
     <t>FOLDER\Mainfolder\Remediation_or_Justification Evidence\1-09-2020\RandomFolder1\</t>
   </si>
   <si>
@@ -306,19 +267,43 @@
     <t>FOLDER\Mainfolder\Remediation_or_Justification Evidence\1-22-2020\RandomFolder2\</t>
   </si>
   <si>
-    <t>FOLDER\Mainfolder\Remediation_or_Justification Evidence\1-22-2020\CHR0000391114.pdf</t>
-  </si>
-  <si>
-    <t>FOLDER\Mainfolder\Remediation_or_Justification Evidence\1-22-2020\RE: Random Email.msg</t>
-  </si>
-  <si>
     <t>FOLDER\Mainfolder\Remediation_or_Justification Evidence\1-24-2020\CHR0000381057.pdf</t>
   </si>
   <si>
     <t>FOLDER\Mainfolder\Remediation_or_Justification Evidence\1-24-2020\CHR0000382957.pdf</t>
   </si>
   <si>
-    <t>FOLDER\Mainfolder\Remediation_or_Justification Evidence\1-24-2020\RE: Random Email.msg</t>
+    <t>something</t>
+  </si>
+  <si>
+    <t>Invalid</t>
+  </si>
+  <si>
+    <t>CHANGES - MissingFromFolders oiuer3298.txt_07.01.73.eml</t>
+  </si>
+  <si>
+    <t>\\MainFolder\Daily_Change_Monitoring\1Jan2019\1-24-2020\CHANGES - MissingFromFolders oiuer3298.txt_07.01.73.eml</t>
+  </si>
+  <si>
+    <t>missing_server</t>
+  </si>
+  <si>
+    <t>RE: Random Email missing.msg</t>
+  </si>
+  <si>
+    <t>FOLDER\Mainfolder\Remediation_or_Justification Evidence\Invalid Folder\1-14-2020\CHR0000291924.pdf</t>
+  </si>
+  <si>
+    <t>FOLDER\Mainfolder\Remediation_or_Justification Evidence\1-09-2020\RE Random Email.msg</t>
+  </si>
+  <si>
+    <t>FOLDER\Mainfolder\Remediation_or_Justification Evidence\1-14-2020\RE Random Email.msg</t>
+  </si>
+  <si>
+    <t>FOLDER\Mainfolder\Remediation_or_Justification Evidence\1-22-2020\RE Random Email missing.msg</t>
+  </si>
+  <si>
+    <t>FOLDER\Mainfolder\Remediation_or_Justification Evidence\1-24-2020\RE Random Email.msg</t>
   </si>
 </sst>
 </file>
@@ -686,30 +671,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M120"/>
+  <dimension ref="A1:M118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="11.6328125" customWidth="1"/>
-    <col min="2" max="2" width="15.36328125" customWidth="1"/>
-    <col min="3" max="3" width="15.453125" customWidth="1"/>
+    <col min="1" max="1" width="11.62890625" customWidth="1"/>
+    <col min="2" max="2" width="15.3671875" customWidth="1"/>
+    <col min="3" max="3" width="15.47265625" customWidth="1"/>
     <col min="4" max="4" width="61" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.36328125" customWidth="1"/>
-    <col min="6" max="6" width="17.6328125" customWidth="1"/>
-    <col min="7" max="7" width="18.453125" customWidth="1"/>
+    <col min="5" max="5" width="77.5234375" customWidth="1"/>
+    <col min="6" max="6" width="17.62890625" customWidth="1"/>
+    <col min="7" max="7" width="18.47265625" customWidth="1"/>
     <col min="8" max="8" width="22" customWidth="1"/>
-    <col min="9" max="9" width="21.453125" customWidth="1"/>
+    <col min="9" max="9" width="21.47265625" customWidth="1"/>
     <col min="10" max="10" width="11" customWidth="1"/>
     <col min="11" max="11" width="29" customWidth="1"/>
-    <col min="12" max="12" width="92.453125" customWidth="1"/>
+    <col min="12" max="12" width="92.47265625" customWidth="1"/>
     <col min="13" max="13" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="55.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" ht="54.9" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -750,647 +735,651 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="8">
         <v>43839</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="M2" s="10"/>
-    </row>
-    <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+      <c r="M2" s="10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="8">
         <v>43839</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="M3" s="10"/>
-    </row>
-    <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+      <c r="M3" s="10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="8">
         <v>43839</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="G4" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" s="10" t="s">
-        <v>72</v>
-      </c>
       <c r="J4" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="K4" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="K4" s="4" t="s">
-        <v>84</v>
-      </c>
       <c r="L4" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="M4" s="10"/>
-    </row>
-    <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>77</v>
+      </c>
+      <c r="M4" s="10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="8">
         <v>43839</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I5" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="K5" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="J5" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>83</v>
-      </c>
       <c r="L5" s="7" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="M5" s="10"/>
     </row>
-    <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="8">
         <v>43843</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I6" s="10" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="L6" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="M6" s="10"/>
-    </row>
-    <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+      <c r="M6" s="10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="8">
         <v>43843</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I7" s="10" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="K7" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="M7" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="L7" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="M7" s="10"/>
-    </row>
-    <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="8">
         <v>43843</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="L8" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="M8" s="10"/>
-    </row>
-    <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>76</v>
+      </c>
+      <c r="M8" s="10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="8">
         <v>43844</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C9" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="H9" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>20</v>
-      </c>
       <c r="I9" s="10" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="L9" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="M9" s="10"/>
-    </row>
-    <row r="10" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+      <c r="M9" s="10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="8">
         <v>43844</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="L10" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="M10" s="10"/>
-    </row>
-    <row r="11" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>88</v>
+      </c>
+      <c r="M10" s="10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="8">
         <v>43852</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F11" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I11" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="G11" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I11" s="11" t="s">
-        <v>68</v>
-      </c>
       <c r="J11" s="10" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="K11" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="L11" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="L11" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="M11" s="10"/>
-    </row>
-    <row r="12" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="M11" s="10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="8">
         <v>43852</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E12" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I12" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="J12" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="L12" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="M12" s="10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="8">
+        <v>43854</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I13" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="J13" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="K13" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="L13" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="M13" s="10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="8">
+        <v>43854</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F12" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="G12" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="I12" s="11" t="s">
+      <c r="C14" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I14" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="J14" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="K14" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="J12" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="K12" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="L12" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="M12" s="10"/>
-    </row>
-    <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="8">
-        <v>43852</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="G13" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I13" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="J13" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="K13" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="L13" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="M13" s="10"/>
-    </row>
-    <row r="14" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="8">
-        <v>43852</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F14" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="G14" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="I14" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="J14" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="K14" s="4" t="s">
-        <v>75</v>
-      </c>
       <c r="L14" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="M14" s="10"/>
-    </row>
-    <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>81</v>
+      </c>
+      <c r="M14" s="10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="8">
         <v>43854</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E15" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I15" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="F15" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="G15" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I15" s="11" t="s">
+      <c r="J15" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="J15" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="K15" s="5" t="s">
-        <v>77</v>
+      <c r="K15" s="4" t="s">
+        <v>66</v>
       </c>
       <c r="L15" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="M15" s="10"/>
-    </row>
-    <row r="16" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>92</v>
+      </c>
+      <c r="M15" s="10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="8">
         <v>43854</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>61</v>
+      <c r="B16" s="4" t="s">
+        <v>55</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>42</v>
+        <v>84</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>58</v>
+        <v>85</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="I16" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="I16" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="J16" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="K16" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="J16" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="K16" s="5" t="s">
-        <v>76</v>
-      </c>
       <c r="L16" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="M16" s="10"/>
-    </row>
-    <row r="17" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="8">
-        <v>43854</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="F17" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="G17" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="I17" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="J17" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="K17" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="L17" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="M17" s="10"/>
-    </row>
-    <row r="18" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="12"/>
+        <v>92</v>
+      </c>
+      <c r="M16" s="10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="12"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
-      <c r="E18" s="5"/>
+      <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
-      <c r="L18" s="5"/>
+      <c r="L18" s="2"/>
       <c r="M18" s="2"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A19" s="12"/>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
@@ -1402,9 +1391,8 @@
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -1417,9 +1405,8 @@
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -1433,7 +1420,7 @@
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -1447,7 +1434,7 @@
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -1461,7 +1448,7 @@
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -1475,7 +1462,7 @@
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -1489,7 +1476,7 @@
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -1503,7 +1490,7 @@
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -1517,7 +1504,7 @@
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -1531,7 +1518,7 @@
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -1545,7 +1532,7 @@
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -1559,7 +1546,7 @@
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -1573,7 +1560,7 @@
       <c r="K31" s="2"/>
       <c r="L31" s="2"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -1587,7 +1574,7 @@
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -1601,7 +1588,7 @@
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -1615,7 +1602,7 @@
       <c r="K34" s="2"/>
       <c r="L34" s="2"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -1629,7 +1616,7 @@
       <c r="K35" s="2"/>
       <c r="L35" s="2"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -1643,7 +1630,7 @@
       <c r="K36" s="2"/>
       <c r="L36" s="2"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -1657,7 +1644,7 @@
       <c r="K37" s="2"/>
       <c r="L37" s="2"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -1671,7 +1658,7 @@
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -1685,7 +1672,7 @@
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -1699,7 +1686,7 @@
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -1713,7 +1700,7 @@
       <c r="K41" s="2"/>
       <c r="L41" s="2"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -1727,7 +1714,7 @@
       <c r="K42" s="2"/>
       <c r="L42" s="2"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -1741,7 +1728,7 @@
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -1755,7 +1742,7 @@
       <c r="K44" s="2"/>
       <c r="L44" s="2"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -1769,7 +1756,7 @@
       <c r="K45" s="2"/>
       <c r="L45" s="2"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -1783,7 +1770,7 @@
       <c r="K46" s="2"/>
       <c r="L46" s="2"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -1797,7 +1784,7 @@
       <c r="K47" s="2"/>
       <c r="L47" s="2"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -1811,7 +1798,7 @@
       <c r="K48" s="2"/>
       <c r="L48" s="2"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -1825,7 +1812,7 @@
       <c r="K49" s="2"/>
       <c r="L49" s="2"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
@@ -1839,7 +1826,7 @@
       <c r="K50" s="2"/>
       <c r="L50" s="2"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
@@ -1853,7 +1840,7 @@
       <c r="K51" s="2"/>
       <c r="L51" s="2"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
@@ -1867,7 +1854,7 @@
       <c r="K52" s="2"/>
       <c r="L52" s="2"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
@@ -1881,7 +1868,7 @@
       <c r="K53" s="2"/>
       <c r="L53" s="2"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
@@ -1895,7 +1882,7 @@
       <c r="K54" s="2"/>
       <c r="L54" s="2"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
@@ -1909,7 +1896,7 @@
       <c r="K55" s="2"/>
       <c r="L55" s="2"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
@@ -1923,7 +1910,7 @@
       <c r="K56" s="2"/>
       <c r="L56" s="2"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
@@ -1937,7 +1924,7 @@
       <c r="K57" s="2"/>
       <c r="L57" s="2"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
@@ -1951,7 +1938,7 @@
       <c r="K58" s="2"/>
       <c r="L58" s="2"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
@@ -1965,7 +1952,7 @@
       <c r="K59" s="2"/>
       <c r="L59" s="2"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
@@ -1979,7 +1966,7 @@
       <c r="K60" s="2"/>
       <c r="L60" s="2"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
@@ -1993,7 +1980,7 @@
       <c r="K61" s="2"/>
       <c r="L61" s="2"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
@@ -2007,7 +1994,7 @@
       <c r="K62" s="2"/>
       <c r="L62" s="2"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
@@ -2021,7 +2008,7 @@
       <c r="K63" s="2"/>
       <c r="L63" s="2"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
@@ -2035,7 +2022,7 @@
       <c r="K64" s="2"/>
       <c r="L64" s="2"/>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
@@ -2049,7 +2036,7 @@
       <c r="K65" s="2"/>
       <c r="L65" s="2"/>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
@@ -2063,7 +2050,7 @@
       <c r="K66" s="2"/>
       <c r="L66" s="2"/>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
@@ -2077,7 +2064,7 @@
       <c r="K67" s="2"/>
       <c r="L67" s="2"/>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
@@ -2091,7 +2078,7 @@
       <c r="K68" s="2"/>
       <c r="L68" s="2"/>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
@@ -2105,7 +2092,7 @@
       <c r="K69" s="2"/>
       <c r="L69" s="2"/>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="2"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
@@ -2119,7 +2106,7 @@
       <c r="K70" s="2"/>
       <c r="L70" s="2"/>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
@@ -2133,7 +2120,7 @@
       <c r="K71" s="2"/>
       <c r="L71" s="2"/>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
@@ -2147,7 +2134,7 @@
       <c r="K72" s="2"/>
       <c r="L72" s="2"/>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
@@ -2161,7 +2148,7 @@
       <c r="K73" s="2"/>
       <c r="L73" s="2"/>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
@@ -2175,7 +2162,7 @@
       <c r="K74" s="2"/>
       <c r="L74" s="2"/>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
@@ -2189,7 +2176,7 @@
       <c r="K75" s="2"/>
       <c r="L75" s="2"/>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
@@ -2203,7 +2190,7 @@
       <c r="K76" s="2"/>
       <c r="L76" s="2"/>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="2"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
@@ -2217,7 +2204,7 @@
       <c r="K77" s="2"/>
       <c r="L77" s="2"/>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="2"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
@@ -2231,7 +2218,7 @@
       <c r="K78" s="2"/>
       <c r="L78" s="2"/>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="2"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
@@ -2245,7 +2232,7 @@
       <c r="K79" s="2"/>
       <c r="L79" s="2"/>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="2"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
@@ -2259,7 +2246,7 @@
       <c r="K80" s="2"/>
       <c r="L80" s="2"/>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="2"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
@@ -2273,7 +2260,7 @@
       <c r="K81" s="2"/>
       <c r="L81" s="2"/>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
@@ -2287,7 +2274,7 @@
       <c r="K82" s="2"/>
       <c r="L82" s="2"/>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
@@ -2301,7 +2288,7 @@
       <c r="K83" s="2"/>
       <c r="L83" s="2"/>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" s="2"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
@@ -2315,7 +2302,7 @@
       <c r="K84" s="2"/>
       <c r="L84" s="2"/>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" s="2"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
@@ -2329,7 +2316,7 @@
       <c r="K85" s="2"/>
       <c r="L85" s="2"/>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" s="2"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
@@ -2343,7 +2330,7 @@
       <c r="K86" s="2"/>
       <c r="L86" s="2"/>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" s="2"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
@@ -2357,7 +2344,7 @@
       <c r="K87" s="2"/>
       <c r="L87" s="2"/>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" s="2"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
@@ -2371,7 +2358,7 @@
       <c r="K88" s="2"/>
       <c r="L88" s="2"/>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" s="2"/>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
@@ -2385,7 +2372,7 @@
       <c r="K89" s="2"/>
       <c r="L89" s="2"/>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" s="2"/>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
@@ -2399,7 +2386,7 @@
       <c r="K90" s="2"/>
       <c r="L90" s="2"/>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" s="2"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
@@ -2413,7 +2400,7 @@
       <c r="K91" s="2"/>
       <c r="L91" s="2"/>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" s="2"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
@@ -2427,7 +2414,7 @@
       <c r="K92" s="2"/>
       <c r="L92" s="2"/>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" s="2"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
@@ -2441,7 +2428,7 @@
       <c r="K93" s="2"/>
       <c r="L93" s="2"/>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" s="2"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
@@ -2455,7 +2442,7 @@
       <c r="K94" s="2"/>
       <c r="L94" s="2"/>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" s="2"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
@@ -2469,7 +2456,7 @@
       <c r="K95" s="2"/>
       <c r="L95" s="2"/>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" s="2"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
@@ -2483,7 +2470,7 @@
       <c r="K96" s="2"/>
       <c r="L96" s="2"/>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" s="2"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
@@ -2497,7 +2484,7 @@
       <c r="K97" s="2"/>
       <c r="L97" s="2"/>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" s="2"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
@@ -2511,7 +2498,7 @@
       <c r="K98" s="2"/>
       <c r="L98" s="2"/>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" s="2"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
@@ -2525,7 +2512,7 @@
       <c r="K99" s="2"/>
       <c r="L99" s="2"/>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" s="2"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
@@ -2539,7 +2526,7 @@
       <c r="K100" s="2"/>
       <c r="L100" s="2"/>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" s="2"/>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
@@ -2553,7 +2540,7 @@
       <c r="K101" s="2"/>
       <c r="L101" s="2"/>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" s="2"/>
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
@@ -2567,7 +2554,7 @@
       <c r="K102" s="2"/>
       <c r="L102" s="2"/>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" s="2"/>
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
@@ -2581,7 +2568,7 @@
       <c r="K103" s="2"/>
       <c r="L103" s="2"/>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" s="2"/>
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
@@ -2595,7 +2582,7 @@
       <c r="K104" s="2"/>
       <c r="L104" s="2"/>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" s="2"/>
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
@@ -2609,7 +2596,7 @@
       <c r="K105" s="2"/>
       <c r="L105" s="2"/>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" s="2"/>
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
@@ -2623,7 +2610,7 @@
       <c r="K106" s="2"/>
       <c r="L106" s="2"/>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" s="2"/>
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
@@ -2637,7 +2624,7 @@
       <c r="K107" s="2"/>
       <c r="L107" s="2"/>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" s="2"/>
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
@@ -2651,7 +2638,7 @@
       <c r="K108" s="2"/>
       <c r="L108" s="2"/>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" s="2"/>
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
@@ -2665,7 +2652,7 @@
       <c r="K109" s="2"/>
       <c r="L109" s="2"/>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" s="2"/>
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
@@ -2679,7 +2666,7 @@
       <c r="K110" s="2"/>
       <c r="L110" s="2"/>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" s="2"/>
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
@@ -2693,7 +2680,7 @@
       <c r="K111" s="2"/>
       <c r="L111" s="2"/>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" s="2"/>
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
@@ -2707,7 +2694,7 @@
       <c r="K112" s="2"/>
       <c r="L112" s="2"/>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" s="2"/>
       <c r="B113" s="2"/>
       <c r="C113" s="2"/>
@@ -2721,7 +2708,7 @@
       <c r="K113" s="2"/>
       <c r="L113" s="2"/>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" s="2"/>
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
@@ -2735,7 +2722,7 @@
       <c r="K114" s="2"/>
       <c r="L114" s="2"/>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" s="2"/>
       <c r="B115" s="2"/>
       <c r="C115" s="2"/>
@@ -2749,7 +2736,7 @@
       <c r="K115" s="2"/>
       <c r="L115" s="2"/>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A116" s="2"/>
       <c r="B116" s="2"/>
       <c r="C116" s="2"/>
@@ -2763,7 +2750,7 @@
       <c r="K116" s="2"/>
       <c r="L116" s="2"/>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A117" s="2"/>
       <c r="B117" s="2"/>
       <c r="C117" s="2"/>
@@ -2777,7 +2764,7 @@
       <c r="K117" s="2"/>
       <c r="L117" s="2"/>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A118" s="2"/>
       <c r="B118" s="2"/>
       <c r="C118" s="2"/>
@@ -2791,34 +2778,6 @@
       <c r="K118" s="2"/>
       <c r="L118" s="2"/>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A119" s="2"/>
-      <c r="B119" s="2"/>
-      <c r="C119" s="2"/>
-      <c r="D119" s="2"/>
-      <c r="E119" s="2"/>
-      <c r="F119" s="2"/>
-      <c r="G119" s="2"/>
-      <c r="H119" s="2"/>
-      <c r="I119" s="2"/>
-      <c r="J119" s="2"/>
-      <c r="K119" s="2"/>
-      <c r="L119" s="2"/>
-    </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A120" s="2"/>
-      <c r="B120" s="2"/>
-      <c r="C120" s="2"/>
-      <c r="D120" s="2"/>
-      <c r="E120" s="2"/>
-      <c r="F120" s="2"/>
-      <c r="G120" s="2"/>
-      <c r="H120" s="2"/>
-      <c r="I120" s="2"/>
-      <c r="J120" s="2"/>
-      <c r="K120" s="2"/>
-      <c r="L120" s="2"/>
-    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -2827,36 +2786,34 @@
     <hyperlink ref="E9" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
     <hyperlink ref="E10" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
     <hyperlink ref="E11" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="E12:E14" r:id="rId7" display="\\MainFolder\Daily_Change_Monitoring\1Jan2019\1-22-2020\" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="E16" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="E15" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="E17" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="E12" r:id="rId7" display="\\MainFolder\Daily_Change_Monitoring\1Jan2019\1-22-2020\" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="E14" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="E13" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="E15" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
     <hyperlink ref="E3" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
     <hyperlink ref="E4" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
     <hyperlink ref="E5" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
     <hyperlink ref="E7" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
     <hyperlink ref="E8" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="E12" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="E13" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="E14" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="L2" r:id="rId19" display="\\MainFolder\Remediation_or_Justification Evidence\1-09-2020\RE: Random Email.msg" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="L6" r:id="rId20" display="\\MainFolder\Remediation_or_Justification Evidence\1-09-2020\RE: Random Email.msg" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="L9" r:id="rId21" display="\\MainFolder\Remediation_or_Justification Evidence\1-14-2020\RE: Random Email.msg" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="L14" r:id="rId22" display="\\MainFolder\Remediation_or_Justification Evidence\1-22-2020\RE: Random Email.msg" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="L17" r:id="rId23" display="\\MainFolder\Remediation_or_Justification Evidence\1-24-2020\RE: Random Email.msg" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="L13" r:id="rId24" display="\\MainFolder\Remediation_or_Justification Evidence\1-22-2020\RE: Random Email.msg" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="L4" r:id="rId25" display="\\MainFolder\Remediation_or_Justification Evidence\1-09-2020\RandomFolder1\" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="L5" r:id="rId26" display="\\MainFolder\Remediation_or_Justification Evidence\1-09-2020\CHR0000928476.pdf" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="L7" r:id="rId27" display="\\MainFolder\Remediation_or_Justification Evidence\1-13-2020\CHR0000230943.pdf" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="L8" r:id="rId28" display="\\MainFolder\Remediation_or_Justification Evidence\1-13-2020\CHR0000123095.pdf" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="L10" r:id="rId29" display="\\MainFolder\Remediation_or_Justification Evidence\1-14-2020\CHR0000291924.pdf" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="L11:L12" r:id="rId30" display="\\MainFolder\Remediation_or_Justification Evidence\1-22-2020\RE: Random Email.msg" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="L11" r:id="rId31" display="\\MainFolder\Remediation_or_Justification Evidence\1-22-2020\RandomFolder2\" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="L12" r:id="rId32" display="\\MainFolder\Remediation_or_Justification Evidence\1-22-2020\CHR0000391114.pdf" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="L15:L16" r:id="rId33" display="\\MainFolder\Remediation_or_Justification Evidence\1-24-2020\RE: Random Email.msg" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="L15" r:id="rId34" display="\\MainFolder\Remediation_or_Justification Evidence\1-24-2020\CHR0000381057.pdf" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="L16" r:id="rId35" display="\\MainFolder\Remediation_or_Justification Evidence\1-24-2020\CHR0000382957.pdf" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="L3" r:id="rId36" display="\\MainFolder\Remediation_or_Justification Evidence\1-09-2020\RE: Random Email.msg" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="E12" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="L2" r:id="rId17" display="\\MainFolder\Remediation_or_Justification Evidence\1-09-2020\RE: Random Email.msg" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="L6" r:id="rId18" display="\\MainFolder\Remediation_or_Justification Evidence\1-09-2020\RE: Random Email.msg" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="L9" r:id="rId19" display="\\MainFolder\Remediation_or_Justification Evidence\1-14-2020\RE: Random Email.msg" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="L12" r:id="rId20" display="\\MainFolder\Remediation_or_Justification Evidence\1-22-2020\RE: Random Email.msg" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="L15" r:id="rId21" display="\\MainFolder\Remediation_or_Justification Evidence\1-24-2020\RE: Random Email.msg" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="L4" r:id="rId22" display="\\MainFolder\Remediation_or_Justification Evidence\1-09-2020\RandomFolder1\" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="L5" r:id="rId23" display="\\MainFolder\Remediation_or_Justification Evidence\1-09-2020\CHR0000928476.pdf" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="L7" r:id="rId24" display="\\MainFolder\Remediation_or_Justification Evidence\1-13-2020\CHR0000230943.pdf" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="L8" r:id="rId25" display="\\MainFolder\Remediation_or_Justification Evidence\1-13-2020\CHR0000123095.pdf" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="L10" r:id="rId26" display="\\MainFolder\Remediation_or_Justification Evidence\1-14-2020\CHR0000291924.pdf" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="L11" r:id="rId27" display="\\MainFolder\Remediation_or_Justification Evidence\1-22-2020\RE: Random Email.msg" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="L11" r:id="rId28" display="\\MainFolder\Remediation_or_Justification Evidence\1-22-2020\RandomFolder2\" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="L13:L14" r:id="rId29" display="\\MainFolder\Remediation_or_Justification Evidence\1-24-2020\RE: Random Email.msg" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="L13" r:id="rId30" display="\\MainFolder\Remediation_or_Justification Evidence\1-24-2020\CHR0000381057.pdf" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="L14" r:id="rId31" display="\\MainFolder\Remediation_or_Justification Evidence\1-24-2020\CHR0000382957.pdf" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="L3" r:id="rId32" display="\\MainFolder\Remediation_or_Justification Evidence\1-09-2020\RE: Random Email.msg" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="E16" r:id="rId33" xr:uid="{64586501-B352-4FCB-A33E-6BC1F8C98BC3}"/>
+    <hyperlink ref="L16" r:id="rId34" display="\\MainFolder\Remediation_or_Justification Evidence\1-24-2020\RE: Random Email.msg" xr:uid="{7AADC3FF-F4AF-4D4B-B372-93D0BBB254DF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added filter data table activity to ValidateRandomDaysWithServer and added a for each activity to check for the Email in Findings Tracker Missing From Folders Business Exception
</commit_message>
<xml_diff>
--- a/FOLDER/Mainfolder/Daily_Change_Monitoring/Findings Tracker.xlsx
+++ b/FOLDER/Mainfolder/Daily_Change_Monitoring/Findings Tracker.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dylan\Documents\UiPath\Robotic_Process_Automation\FOLDER\Mainfolder\Daily_Change_Monitoring\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S\Documents\UiPath_2\Robotic_Process_Automation\FOLDER\Mainfolder\Daily_Change_Monitoring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01FACFA0-F1A8-47AF-ACBF-B45487FA8935}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D27785F7-8857-430D-9A8F-AA12F3FCC2FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FindingsTracker" sheetId="1" r:id="rId1"/>
@@ -144,48 +144,6 @@
     <t>CHANGES - SOX Audit Report for oiuer3298.txt_07.01.73.eml</t>
   </si>
   <si>
-    <t>\\MainFolder\Daily_Change_Monitoring\1Jan2019\1-09-2020\CHANGES - SOX Audit Report for magic_qq_appl.txt_07.01.73.eml</t>
-  </si>
-  <si>
-    <t>\\MainFolder\Daily_Change_Monitoring\1Jan2019\1-09-2020\CHANGES - SOX Audit Report for testps01.txt_07.01.73.eml</t>
-  </si>
-  <si>
-    <t>\\MainFolder\Daily_Change_Monitoring\1Jan2019\1-09-2020\CHANGES - SOX Audit Report for testps0324.txt_07.01.73.eml</t>
-  </si>
-  <si>
-    <t>\\MainFolder\Daily_Change_Monitoring\1Jan2019\1-09-2020\CHANGES - SOX Audit Report for testps9023.txt_07.01.73.eml</t>
-  </si>
-  <si>
-    <t>\\MainFolder\Daily_Change_Monitoring\1Jan2019\1-13-2020\CHANGES - SOX Audit Report for magic_kl02.txt_07.01.73.eml</t>
-  </si>
-  <si>
-    <t>\\MainFolder\Daily_Change_Monitoring\1Jan2019\1-13-2020\CHANGES - SOX Audit Report for magic_kq_023.txt_07.01.73.eml</t>
-  </si>
-  <si>
-    <t>\\MainFolder\Daily_Change_Monitoring\1Jan2019\1-13-2020\CHANGES - SOX Audit Report for magic_qq_appl.txt_07.01.73.eml</t>
-  </si>
-  <si>
-    <t>\\MainFolder\Daily_Change_Monitoring\1Jan2019\1-14-2020\CHANGES - SOX Audit Report for magic9023.txt_07.01.73.eml</t>
-  </si>
-  <si>
-    <t>\\MainFolder\Daily_Change_Monitoring\1Jan2019\1-14-2020\CHANGES - SOX Audit Report for magic9843.txt_07.01.73.eml</t>
-  </si>
-  <si>
-    <t>\\MainFolder\Daily_Change_Monitoring\1Jan2019\1-22-2020\CHANGES - SOX Audit Report for magic435.txt_07.01.73.eml</t>
-  </si>
-  <si>
-    <t>\\MainFolder\Daily_Change_Monitoring\1Jan2019\1-22-2020\CHANGES - SOX Audit Report for test234234.txt_07.01.73.eml</t>
-  </si>
-  <si>
-    <t>\\MainFolder\Daily_Change_Monitoring\1Jan2019\1-24-2020\CHANGES - SOX Audit Report for magic_iq23.txt_07.01.73.eml</t>
-  </si>
-  <si>
-    <t>\\MainFolder\Daily_Change_Monitoring\1Jan2019\1-24-2020\CHANGES - SOX Audit Report for testqcl12.txt_07.01.73.eml</t>
-  </si>
-  <si>
-    <t>\\MainFolder\Daily_Change_Monitoring\1Jan2019\1-24-2020\CHANGES - SOX Audit Report for oiuer3298.txt_07.01.73.eml</t>
-  </si>
-  <si>
     <t>ignore</t>
   </si>
   <si>
@@ -282,9 +240,6 @@
     <t>CHANGES - MissingFromFolders oiuer3298.txt_07.01.73.eml</t>
   </si>
   <si>
-    <t>\\MainFolder\Daily_Change_Monitoring\1Jan2019\1-24-2020\CHANGES - MissingFromFolders oiuer3298.txt_07.01.73.eml</t>
-  </si>
-  <si>
     <t>missing_server</t>
   </si>
   <si>
@@ -304,6 +259,51 @@
   </si>
   <si>
     <t>FOLDER\Mainfolder\Remediation_or_Justification Evidence\1-24-2020\RE Random Email.msg</t>
+  </si>
+  <si>
+    <t>FOLDER\Mainfolder\Daily_Change_Monitoring\1Jan2020\1-09-2020\CHANGES - SOX Audit Report for magic_qq_appl.txt_07.01.73.eml</t>
+  </si>
+  <si>
+    <t>FOLDER\Mainfolder\Daily_Change_Monitoring\1Jan2020\1-09-2020\CHANGES - SOX Audit Report for testps01.txt_07.01.73.eml</t>
+  </si>
+  <si>
+    <t>FOLDER\Mainfolder\Daily_Change_Monitoring\1Jan2020\1-09-2020\CHANGES - SOX Audit Report for testps0324.txt_07.01.73.eml</t>
+  </si>
+  <si>
+    <t>FOLDER\Mainfolder\Daily_Change_Monitoring\1Jan2020\1-09-2020\CHANGES - SOX Audit Report for testps9023.txt_07.01.73.eml</t>
+  </si>
+  <si>
+    <t>FOLDER\Mainfolder\Daily_Change_Monitoring\1Jan2020\1-13-2020\CHANGES - SOX Audit Report for magic_kl02.txt_07.01.73.eml</t>
+  </si>
+  <si>
+    <t>FOLDER\Mainfolder\Daily_Change_Monitoring\1Jan2020\1-13-2020\CHANGES - SOX Audit Report for magic_kq_023.txt_07.01.73.eml</t>
+  </si>
+  <si>
+    <t>FOLDER\Mainfolder\Daily_Change_Monitoring\1Jan2020\1-13-2020\CHANGES - SOX Audit Report for magic_qq_appl.txt_07.01.73.eml</t>
+  </si>
+  <si>
+    <t>FOLDER\Mainfolder\Daily_Change_Monitoring\1Jan2020\1-14-2020\CHANGES - SOX Audit Report for magic9023.txt_07.01.73.eml</t>
+  </si>
+  <si>
+    <t>FOLDER\Mainfolder\Daily_Change_Monitoring\1Jan2020\1-14-2020\CHANGES - SOX Audit Report for magic9843.txt_07.01.73.eml</t>
+  </si>
+  <si>
+    <t>FOLDER\Mainfolder\Daily_Change_Monitoring\1Jan2020\1-22-2020\CHANGES - SOX Audit Report for magic435.txt_07.01.73.eml</t>
+  </si>
+  <si>
+    <t>FOLDER\Mainfolder\Daily_Change_Monitoring\1Jan2020\1-22-2020\CHANGES - SOX Audit Report for test234234.txt_07.01.73.eml</t>
+  </si>
+  <si>
+    <t>FOLDER\Mainfolder\Daily_Change_Monitoring\1Jan2020\1-24-2020\CHANGES - SOX Audit Report for magic_iq23.txt_07.01.73.eml</t>
+  </si>
+  <si>
+    <t>FOLDER\Mainfolder\Daily_Change_Monitoring\1Jan2020\1-24-2020\CHANGES - SOX Audit Report for testqcl12.txt_07.01.73.eml</t>
+  </si>
+  <si>
+    <t>FOLDER\Mainfolder\Daily_Change_Monitoring\1Jan2020\1-24-2020\CHANGES - SOX Audit Report for oiuer3298.txt_07.01.73.eml</t>
+  </si>
+  <si>
+    <t>FOLDER\Mainfolder\Daily_Change_Monitoring\1Jan2020\1-24-2020\CHANGES - MissingFromFolders oiuer3298.txt_07.01.73.eml</t>
   </si>
 </sst>
 </file>
@@ -673,28 +673,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.62890625" customWidth="1"/>
-    <col min="2" max="2" width="15.3671875" customWidth="1"/>
-    <col min="3" max="3" width="15.47265625" customWidth="1"/>
-    <col min="4" max="4" width="61" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="77.5234375" customWidth="1"/>
-    <col min="6" max="6" width="17.62890625" customWidth="1"/>
-    <col min="7" max="7" width="18.47265625" customWidth="1"/>
+    <col min="1" max="1" width="11.6328125" customWidth="1"/>
+    <col min="2" max="2" width="15.36328125" customWidth="1"/>
+    <col min="3" max="3" width="15.453125" customWidth="1"/>
+    <col min="4" max="4" width="31.08984375" customWidth="1"/>
+    <col min="5" max="5" width="54.81640625" customWidth="1"/>
+    <col min="6" max="6" width="17.6328125" customWidth="1"/>
+    <col min="7" max="7" width="18.453125" customWidth="1"/>
     <col min="8" max="8" width="22" customWidth="1"/>
-    <col min="9" max="9" width="21.47265625" customWidth="1"/>
+    <col min="9" max="9" width="21.453125" customWidth="1"/>
     <col min="10" max="10" width="11" customWidth="1"/>
     <col min="11" max="11" width="29" customWidth="1"/>
-    <col min="12" max="12" width="92.47265625" customWidth="1"/>
+    <col min="12" max="12" width="92.453125" customWidth="1"/>
     <col min="13" max="13" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="54.9" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:13" ht="55.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -735,12 +735,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8">
         <v>43839</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>18</v>
@@ -749,39 +749,39 @@
         <v>26</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>39</v>
+        <v>78</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>17</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="M2" s="10" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="8">
         <v>43839</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>18</v>
@@ -790,39 +790,39 @@
         <v>27</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>40</v>
+        <v>79</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>15</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="M3" s="10" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="8">
         <v>43839</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>18</v>
@@ -831,39 +831,39 @@
         <v>28</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>14</v>
       </c>
       <c r="I4" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="L4" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="J4" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="L4" s="7" t="s">
-        <v>77</v>
-      </c>
       <c r="M4" s="10" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="8">
         <v>43839</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>18</v>
@@ -872,37 +872,37 @@
         <v>29</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>42</v>
+        <v>81</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>16</v>
       </c>
       <c r="I5" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="L5" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="J5" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="L5" s="7" t="s">
-        <v>78</v>
-      </c>
       <c r="M5" s="10"/>
     </row>
-    <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="8">
         <v>43843</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>18</v>
@@ -911,39 +911,39 @@
         <v>30</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>43</v>
+        <v>82</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="H6" s="4" t="s">
         <v>13</v>
       </c>
       <c r="I6" s="10" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="L6" s="7" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="M6" s="10" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="8">
         <v>43843</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>18</v>
@@ -952,39 +952,39 @@
         <v>31</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>44</v>
+        <v>83</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>14</v>
       </c>
       <c r="I7" s="10" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="L7" s="7" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="M7" s="10" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="8">
         <v>43843</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>18</v>
@@ -993,39 +993,39 @@
         <v>26</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>45</v>
+        <v>84</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="I8" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="J8" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="L8" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="J8" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="K8" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="L8" s="7" t="s">
-        <v>76</v>
-      </c>
       <c r="M8" s="10" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="8">
         <v>43844</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>18</v>
@@ -1034,39 +1034,39 @@
         <v>32</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>46</v>
+        <v>85</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>19</v>
       </c>
       <c r="I9" s="10" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="L9" s="7" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="M9" s="10" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="8">
         <v>43844</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>18</v>
@@ -1075,39 +1075,39 @@
         <v>33</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>47</v>
+        <v>86</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="H10" s="4" t="s">
         <v>20</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="L10" s="7" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="M10" s="10" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="8">
         <v>43852</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>18</v>
@@ -1116,39 +1116,39 @@
         <v>34</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>48</v>
+        <v>87</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="H11" s="4" t="s">
         <v>21</v>
       </c>
       <c r="I11" s="11" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="J11" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="L11" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="K11" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="L11" s="7" t="s">
-        <v>79</v>
-      </c>
       <c r="M11" s="10" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="8">
         <v>43852</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>18</v>
@@ -1157,39 +1157,39 @@
         <v>35</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>49</v>
+        <v>88</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="H12" s="4" t="s">
         <v>22</v>
       </c>
       <c r="I12" s="10" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="L12" s="7" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="M12" s="10" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="8">
         <v>43854</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>18</v>
@@ -1198,39 +1198,39 @@
         <v>36</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>50</v>
+        <v>89</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="H13" s="4" t="s">
         <v>23</v>
       </c>
       <c r="I13" s="11" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="J13" s="10" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="K13" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="L13" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="M13" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="L13" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="M13" s="10" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="14" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="8">
         <v>43854</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>18</v>
@@ -1239,39 +1239,39 @@
         <v>37</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>51</v>
+        <v>90</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="H14" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I14" s="11" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="K14" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="L14" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="L14" s="7" t="s">
-        <v>81</v>
-      </c>
       <c r="M14" s="10" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="8">
         <v>43854</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>18</v>
@@ -1280,75 +1280,75 @@
         <v>38</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>52</v>
+        <v>91</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="H15" s="4" t="s">
         <v>25</v>
       </c>
       <c r="I15" s="10" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="L15" s="7" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="M15" s="10" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="8">
         <v>43854</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="H16" s="4" t="s">
         <v>25</v>
       </c>
       <c r="I16" s="10" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="J16" s="10" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="L16" s="7" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="M16" s="10" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="12"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -1363,7 +1363,7 @@
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -1378,7 +1378,7 @@
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -1392,7 +1392,7 @@
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -1406,7 +1406,7 @@
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -1420,7 +1420,7 @@
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -1434,7 +1434,7 @@
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -1448,7 +1448,7 @@
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -1462,7 +1462,7 @@
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -1476,7 +1476,7 @@
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -1490,7 +1490,7 @@
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -1504,7 +1504,7 @@
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -1518,7 +1518,7 @@
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -1532,7 +1532,7 @@
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -1546,7 +1546,7 @@
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -1560,7 +1560,7 @@
       <c r="K31" s="2"/>
       <c r="L31" s="2"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -1574,7 +1574,7 @@
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -1588,7 +1588,7 @@
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -1602,7 +1602,7 @@
       <c r="K34" s="2"/>
       <c r="L34" s="2"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -1616,7 +1616,7 @@
       <c r="K35" s="2"/>
       <c r="L35" s="2"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -1630,7 +1630,7 @@
       <c r="K36" s="2"/>
       <c r="L36" s="2"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -1644,7 +1644,7 @@
       <c r="K37" s="2"/>
       <c r="L37" s="2"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -1658,7 +1658,7 @@
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -1672,7 +1672,7 @@
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -1686,7 +1686,7 @@
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -1700,7 +1700,7 @@
       <c r="K41" s="2"/>
       <c r="L41" s="2"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -1714,7 +1714,7 @@
       <c r="K42" s="2"/>
       <c r="L42" s="2"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -1728,7 +1728,7 @@
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -1742,7 +1742,7 @@
       <c r="K44" s="2"/>
       <c r="L44" s="2"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -1756,7 +1756,7 @@
       <c r="K45" s="2"/>
       <c r="L45" s="2"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -1770,7 +1770,7 @@
       <c r="K46" s="2"/>
       <c r="L46" s="2"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -1784,7 +1784,7 @@
       <c r="K47" s="2"/>
       <c r="L47" s="2"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -1798,7 +1798,7 @@
       <c r="K48" s="2"/>
       <c r="L48" s="2"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -1812,7 +1812,7 @@
       <c r="K49" s="2"/>
       <c r="L49" s="2"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
@@ -1826,7 +1826,7 @@
       <c r="K50" s="2"/>
       <c r="L50" s="2"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
@@ -1840,7 +1840,7 @@
       <c r="K51" s="2"/>
       <c r="L51" s="2"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
@@ -1854,7 +1854,7 @@
       <c r="K52" s="2"/>
       <c r="L52" s="2"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
@@ -1868,7 +1868,7 @@
       <c r="K53" s="2"/>
       <c r="L53" s="2"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
@@ -1882,7 +1882,7 @@
       <c r="K54" s="2"/>
       <c r="L54" s="2"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
@@ -1896,7 +1896,7 @@
       <c r="K55" s="2"/>
       <c r="L55" s="2"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
@@ -1910,7 +1910,7 @@
       <c r="K56" s="2"/>
       <c r="L56" s="2"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
@@ -1924,7 +1924,7 @@
       <c r="K57" s="2"/>
       <c r="L57" s="2"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
@@ -1938,7 +1938,7 @@
       <c r="K58" s="2"/>
       <c r="L58" s="2"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
@@ -1952,7 +1952,7 @@
       <c r="K59" s="2"/>
       <c r="L59" s="2"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
@@ -1966,7 +1966,7 @@
       <c r="K60" s="2"/>
       <c r="L60" s="2"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
@@ -1980,7 +1980,7 @@
       <c r="K61" s="2"/>
       <c r="L61" s="2"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
@@ -1994,7 +1994,7 @@
       <c r="K62" s="2"/>
       <c r="L62" s="2"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
@@ -2008,7 +2008,7 @@
       <c r="K63" s="2"/>
       <c r="L63" s="2"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
@@ -2022,7 +2022,7 @@
       <c r="K64" s="2"/>
       <c r="L64" s="2"/>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
@@ -2036,7 +2036,7 @@
       <c r="K65" s="2"/>
       <c r="L65" s="2"/>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
@@ -2050,7 +2050,7 @@
       <c r="K66" s="2"/>
       <c r="L66" s="2"/>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
@@ -2064,7 +2064,7 @@
       <c r="K67" s="2"/>
       <c r="L67" s="2"/>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
@@ -2078,7 +2078,7 @@
       <c r="K68" s="2"/>
       <c r="L68" s="2"/>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
@@ -2092,7 +2092,7 @@
       <c r="K69" s="2"/>
       <c r="L69" s="2"/>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A70" s="2"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
@@ -2106,7 +2106,7 @@
       <c r="K70" s="2"/>
       <c r="L70" s="2"/>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
@@ -2120,7 +2120,7 @@
       <c r="K71" s="2"/>
       <c r="L71" s="2"/>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
@@ -2134,7 +2134,7 @@
       <c r="K72" s="2"/>
       <c r="L72" s="2"/>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
@@ -2148,7 +2148,7 @@
       <c r="K73" s="2"/>
       <c r="L73" s="2"/>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
@@ -2162,7 +2162,7 @@
       <c r="K74" s="2"/>
       <c r="L74" s="2"/>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
@@ -2176,7 +2176,7 @@
       <c r="K75" s="2"/>
       <c r="L75" s="2"/>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
@@ -2190,7 +2190,7 @@
       <c r="K76" s="2"/>
       <c r="L76" s="2"/>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A77" s="2"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
@@ -2204,7 +2204,7 @@
       <c r="K77" s="2"/>
       <c r="L77" s="2"/>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A78" s="2"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
@@ -2218,7 +2218,7 @@
       <c r="K78" s="2"/>
       <c r="L78" s="2"/>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A79" s="2"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
@@ -2232,7 +2232,7 @@
       <c r="K79" s="2"/>
       <c r="L79" s="2"/>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A80" s="2"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
@@ -2246,7 +2246,7 @@
       <c r="K80" s="2"/>
       <c r="L80" s="2"/>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A81" s="2"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
@@ -2260,7 +2260,7 @@
       <c r="K81" s="2"/>
       <c r="L81" s="2"/>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
@@ -2274,7 +2274,7 @@
       <c r="K82" s="2"/>
       <c r="L82" s="2"/>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
@@ -2288,7 +2288,7 @@
       <c r="K83" s="2"/>
       <c r="L83" s="2"/>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A84" s="2"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
@@ -2302,7 +2302,7 @@
       <c r="K84" s="2"/>
       <c r="L84" s="2"/>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A85" s="2"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
@@ -2316,7 +2316,7 @@
       <c r="K85" s="2"/>
       <c r="L85" s="2"/>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A86" s="2"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
@@ -2330,7 +2330,7 @@
       <c r="K86" s="2"/>
       <c r="L86" s="2"/>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A87" s="2"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
@@ -2344,7 +2344,7 @@
       <c r="K87" s="2"/>
       <c r="L87" s="2"/>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A88" s="2"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
@@ -2358,7 +2358,7 @@
       <c r="K88" s="2"/>
       <c r="L88" s="2"/>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A89" s="2"/>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
@@ -2372,7 +2372,7 @@
       <c r="K89" s="2"/>
       <c r="L89" s="2"/>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A90" s="2"/>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
@@ -2386,7 +2386,7 @@
       <c r="K90" s="2"/>
       <c r="L90" s="2"/>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A91" s="2"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
@@ -2400,7 +2400,7 @@
       <c r="K91" s="2"/>
       <c r="L91" s="2"/>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A92" s="2"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
@@ -2414,7 +2414,7 @@
       <c r="K92" s="2"/>
       <c r="L92" s="2"/>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A93" s="2"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
@@ -2428,7 +2428,7 @@
       <c r="K93" s="2"/>
       <c r="L93" s="2"/>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A94" s="2"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
@@ -2442,7 +2442,7 @@
       <c r="K94" s="2"/>
       <c r="L94" s="2"/>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A95" s="2"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
@@ -2456,7 +2456,7 @@
       <c r="K95" s="2"/>
       <c r="L95" s="2"/>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A96" s="2"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
@@ -2470,7 +2470,7 @@
       <c r="K96" s="2"/>
       <c r="L96" s="2"/>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A97" s="2"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
@@ -2484,7 +2484,7 @@
       <c r="K97" s="2"/>
       <c r="L97" s="2"/>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A98" s="2"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
@@ -2498,7 +2498,7 @@
       <c r="K98" s="2"/>
       <c r="L98" s="2"/>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A99" s="2"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
@@ -2512,7 +2512,7 @@
       <c r="K99" s="2"/>
       <c r="L99" s="2"/>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A100" s="2"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
@@ -2526,7 +2526,7 @@
       <c r="K100" s="2"/>
       <c r="L100" s="2"/>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A101" s="2"/>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
@@ -2540,7 +2540,7 @@
       <c r="K101" s="2"/>
       <c r="L101" s="2"/>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A102" s="2"/>
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
@@ -2554,7 +2554,7 @@
       <c r="K102" s="2"/>
       <c r="L102" s="2"/>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A103" s="2"/>
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
@@ -2568,7 +2568,7 @@
       <c r="K103" s="2"/>
       <c r="L103" s="2"/>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A104" s="2"/>
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
@@ -2582,7 +2582,7 @@
       <c r="K104" s="2"/>
       <c r="L104" s="2"/>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A105" s="2"/>
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
@@ -2596,7 +2596,7 @@
       <c r="K105" s="2"/>
       <c r="L105" s="2"/>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A106" s="2"/>
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
@@ -2610,7 +2610,7 @@
       <c r="K106" s="2"/>
       <c r="L106" s="2"/>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A107" s="2"/>
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
@@ -2624,7 +2624,7 @@
       <c r="K107" s="2"/>
       <c r="L107" s="2"/>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A108" s="2"/>
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
@@ -2638,7 +2638,7 @@
       <c r="K108" s="2"/>
       <c r="L108" s="2"/>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A109" s="2"/>
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
@@ -2652,7 +2652,7 @@
       <c r="K109" s="2"/>
       <c r="L109" s="2"/>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A110" s="2"/>
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
@@ -2666,7 +2666,7 @@
       <c r="K110" s="2"/>
       <c r="L110" s="2"/>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A111" s="2"/>
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
@@ -2680,7 +2680,7 @@
       <c r="K111" s="2"/>
       <c r="L111" s="2"/>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A112" s="2"/>
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
@@ -2694,7 +2694,7 @@
       <c r="K112" s="2"/>
       <c r="L112" s="2"/>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A113" s="2"/>
       <c r="B113" s="2"/>
       <c r="C113" s="2"/>
@@ -2708,7 +2708,7 @@
       <c r="K113" s="2"/>
       <c r="L113" s="2"/>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A114" s="2"/>
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
@@ -2722,7 +2722,7 @@
       <c r="K114" s="2"/>
       <c r="L114" s="2"/>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A115" s="2"/>
       <c r="B115" s="2"/>
       <c r="C115" s="2"/>
@@ -2736,7 +2736,7 @@
       <c r="K115" s="2"/>
       <c r="L115" s="2"/>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A116" s="2"/>
       <c r="B116" s="2"/>
       <c r="C116" s="2"/>
@@ -2750,7 +2750,7 @@
       <c r="K116" s="2"/>
       <c r="L116" s="2"/>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A117" s="2"/>
       <c r="B117" s="2"/>
       <c r="C117" s="2"/>
@@ -2764,7 +2764,7 @@
       <c r="K117" s="2"/>
       <c r="L117" s="2"/>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A118" s="2"/>
       <c r="B118" s="2"/>
       <c r="C118" s="2"/>
@@ -2780,22 +2780,22 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="E6" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E2" r:id="rId1" display="\\MainFolder\Daily_Change_Monitoring\1Jan2019\1-09-2020\CHANGES - SOX Audit Report for magic_qq_appl.txt_07.01.73.eml" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E6" r:id="rId2" display="\\MainFolder\Daily_Change_Monitoring\1Jan2019\1-13-2020\CHANGES - SOX Audit Report for magic_kl02.txt_07.01.73.eml" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="E7:E8" r:id="rId3" display="\\MainFolder\Daily_Change_Monitoring\1Jan2019\1-13-2020\" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="E9" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="E10" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="E11" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="E9" r:id="rId4" display="\\MainFolder\Daily_Change_Monitoring\1Jan2019\1-14-2020\CHANGES - SOX Audit Report for magic9023.txt_07.01.73.eml" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="E10" r:id="rId5" display="\\MainFolder\Daily_Change_Monitoring\1Jan2019\1-14-2020\CHANGES - SOX Audit Report for magic9843.txt_07.01.73.eml" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="E11" r:id="rId6" display="\\MainFolder\Daily_Change_Monitoring\1Jan2019\1-22-2020\CHANGES - SOX Audit Report for magic435.txt_07.01.73.eml" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
     <hyperlink ref="E12" r:id="rId7" display="\\MainFolder\Daily_Change_Monitoring\1Jan2019\1-22-2020\" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="E14" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="E13" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="E15" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="E3" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="E4" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="E5" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="E7" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="E8" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="E12" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="E14" r:id="rId8" display="\\MainFolder\Daily_Change_Monitoring\1Jan2019\1-24-2020\CHANGES - SOX Audit Report for testqcl12.txt_07.01.73.eml" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="E13" r:id="rId9" display="\\MainFolder\Daily_Change_Monitoring\1Jan2019\1-24-2020\CHANGES - SOX Audit Report for magic_iq23.txt_07.01.73.eml" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="E15" r:id="rId10" display="\\MainFolder\Daily_Change_Monitoring\1Jan2019\1-24-2020\CHANGES - SOX Audit Report for oiuer3298.txt_07.01.73.eml" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="E3" r:id="rId11" display="\\MainFolder\Daily_Change_Monitoring\1Jan2019\1-09-2020\CHANGES - SOX Audit Report for testps01.txt_07.01.73.eml" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="E4" r:id="rId12" display="\\MainFolder\Daily_Change_Monitoring\1Jan2019\1-09-2020\CHANGES - SOX Audit Report for testps0324.txt_07.01.73.eml" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="E5" r:id="rId13" display="\\MainFolder\Daily_Change_Monitoring\1Jan2019\1-09-2020\CHANGES - SOX Audit Report for testps9023.txt_07.01.73.eml" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="E7" r:id="rId14" display="\\MainFolder\Daily_Change_Monitoring\1Jan2019\1-13-2020\CHANGES - SOX Audit Report for magic_kq_023.txt_07.01.73.eml" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="E8" r:id="rId15" display="\\MainFolder\Daily_Change_Monitoring\1Jan2019\1-13-2020\CHANGES - SOX Audit Report for magic_qq_appl.txt_07.01.73.eml" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="E12" r:id="rId16" display="\\MainFolder\Daily_Change_Monitoring\1Jan2019\1-22-2020\CHANGES - SOX Audit Report for test234234.txt_07.01.73.eml" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
     <hyperlink ref="L2" r:id="rId17" display="\\MainFolder\Remediation_or_Justification Evidence\1-09-2020\RE: Random Email.msg" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
     <hyperlink ref="L6" r:id="rId18" display="\\MainFolder\Remediation_or_Justification Evidence\1-09-2020\RE: Random Email.msg" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
     <hyperlink ref="L9" r:id="rId19" display="\\MainFolder\Remediation_or_Justification Evidence\1-14-2020\RE: Random Email.msg" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
@@ -2812,7 +2812,7 @@
     <hyperlink ref="L13" r:id="rId30" display="\\MainFolder\Remediation_or_Justification Evidence\1-24-2020\CHR0000381057.pdf" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
     <hyperlink ref="L14" r:id="rId31" display="\\MainFolder\Remediation_or_Justification Evidence\1-24-2020\CHR0000382957.pdf" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
     <hyperlink ref="L3" r:id="rId32" display="\\MainFolder\Remediation_or_Justification Evidence\1-09-2020\RE: Random Email.msg" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="E16" r:id="rId33" xr:uid="{64586501-B352-4FCB-A33E-6BC1F8C98BC3}"/>
+    <hyperlink ref="E16" r:id="rId33" display="\\MainFolder\Daily_Change_Monitoring\1Jan2019\1-24-2020\CHANGES - MissingFromFolders oiuer3298.txt_07.01.73.eml" xr:uid="{64586501-B352-4FCB-A33E-6BC1F8C98BC3}"/>
     <hyperlink ref="L16" r:id="rId34" display="\\MainFolder\Remediation_or_Justification Evidence\1-24-2020\RE: Random Email.msg" xr:uid="{7AADC3FF-F4AF-4D4B-B372-93D0BBB254DF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>